<commit_message>
Add new speakers, logos and change excel attendees
</commit_message>
<xml_diff>
--- a/images/Attendee Companies Con-X 2022.xlsx
+++ b/images/Attendee Companies Con-X 2022.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
   <si>
     <t>A2 Secure</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Albania Explorer</t>
   </si>
   <si>
+    <t>Allbeds</t>
+  </si>
+  <si>
     <t>Allresnet (Alliance Reservations)</t>
   </si>
   <si>
@@ -64,6 +67,15 @@
     <t>Barcelo Hotel Group</t>
   </si>
   <si>
+    <t>BAVEL-VOXEL GROUP</t>
+  </si>
+  <si>
+    <t>BD Director</t>
+  </si>
+  <si>
+    <t>Bd4 travel</t>
+  </si>
+  <si>
     <t>Belive hotels</t>
   </si>
   <si>
@@ -73,6 +85,9 @@
     <t>Bemyplan</t>
   </si>
   <si>
+    <t>BestDay- HotelDO</t>
+  </si>
+  <si>
     <t>BG Hotels</t>
   </si>
   <si>
@@ -91,6 +106,12 @@
     <t>Clicktrip</t>
   </si>
   <si>
+    <t>ClicnGo</t>
+  </si>
+  <si>
+    <t>Coming2 DMC</t>
+  </si>
+  <si>
     <t>Conector Startup Accelerator</t>
   </si>
   <si>
@@ -118,6 +139,9 @@
     <t>Dieux Travel Service</t>
   </si>
   <si>
+    <t>Director of BD</t>
+  </si>
+  <si>
     <t>Doctorwhatson</t>
   </si>
   <si>
@@ -145,18 +169,24 @@
     <t xml:space="preserve">Euram </t>
   </si>
   <si>
-    <t xml:space="preserve">Expedia Partner Solutions </t>
+    <t>Expedia Partner Solutions</t>
   </si>
   <si>
     <t>Fastpayhotels</t>
   </si>
   <si>
+    <t xml:space="preserve">FDSA </t>
+  </si>
+  <si>
     <t>FI iniciativas</t>
   </si>
   <si>
     <t>FindHotel</t>
   </si>
   <si>
+    <t>Founder</t>
+  </si>
+  <si>
     <t>G2 Travel</t>
   </si>
   <si>
@@ -244,6 +274,9 @@
     <t>iTravex</t>
   </si>
   <si>
+    <t>Jacobs Media Group</t>
+  </si>
+  <si>
     <t>JTB Global Marketing &amp; Travel</t>
   </si>
   <si>
@@ -253,6 +286,9 @@
     <t>Juniper</t>
   </si>
   <si>
+    <t>Kantox</t>
+  </si>
+  <si>
     <t>Karavel</t>
   </si>
   <si>
@@ -316,18 +352,30 @@
     <t>NXOdirect</t>
   </si>
   <si>
+    <t>Ocean Holidays</t>
+  </si>
+  <si>
     <t>Offtryp</t>
   </si>
   <si>
     <t>On the Beach</t>
   </si>
   <si>
+    <t>OnTravel</t>
+  </si>
+  <si>
     <t>Open Destinations</t>
   </si>
   <si>
+    <t>Ostrovok</t>
+  </si>
+  <si>
     <t>OTS Globe</t>
   </si>
   <si>
+    <t>PaynoPain</t>
+  </si>
+  <si>
     <t>PayParc</t>
   </si>
   <si>
@@ -337,6 +385,9 @@
     <t>People of The World</t>
   </si>
   <si>
+    <t>PerfectStay</t>
+  </si>
+  <si>
     <t>Plugandbeds</t>
   </si>
   <si>
@@ -403,6 +454,9 @@
     <t>Smyrooms</t>
   </si>
   <si>
+    <t>Snaptravel</t>
+  </si>
+  <si>
     <t>Solole</t>
   </si>
   <si>
@@ -415,7 +469,7 @@
     <t>Sriggle</t>
   </si>
   <si>
-    <t>Stena Line</t>
+    <t>Stena Line Travel Group</t>
   </si>
   <si>
     <t>Street Life GmbH</t>
@@ -457,6 +511,12 @@
     <t>Travco UK</t>
   </si>
   <si>
+    <t>Travel Weekly Group</t>
+  </si>
+  <si>
+    <t>traveltek</t>
+  </si>
+  <si>
     <t>TravelUp</t>
   </si>
   <si>
@@ -472,6 +532,9 @@
     <t>Tripx Travel AB</t>
   </si>
   <si>
+    <t>Trust My Group</t>
+  </si>
+  <si>
     <t>TUI</t>
   </si>
   <si>
@@ -481,15 +544,15 @@
     <t>Vemsa Travel</t>
   </si>
   <si>
-    <t>Vemsadmc</t>
-  </si>
-  <si>
     <t>Veri Seed Capital</t>
   </si>
   <si>
     <t>Vervotech</t>
   </si>
   <si>
+    <t>Viajes El Corte Ingles</t>
+  </si>
+  <si>
     <t>VIAJES INTERRIAS</t>
   </si>
   <si>
@@ -514,7 +577,7 @@
     <t>Wellnesstraveller</t>
   </si>
   <si>
-    <t>what3words.com</t>
+    <t>what3words</t>
   </si>
   <si>
     <t>WHL/Alba Travel</t>
@@ -536,6 +599,9 @@
   </si>
   <si>
     <t>Zafiro Hotels</t>
+  </si>
+  <si>
+    <t>Zolv</t>
   </si>
   <si>
     <t>Zoopay</t>
@@ -591,6 +657,7 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -600,8 +667,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -853,37 +921,37 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -898,12 +966,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -913,17 +981,17 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -943,7 +1011,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -963,7 +1031,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -978,17 +1046,17 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -998,7 +1066,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1008,22 +1076,22 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1038,32 +1106,32 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1073,17 +1141,17 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1093,7 +1161,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1103,12 +1171,12 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1118,32 +1186,32 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1153,12 +1221,12 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1168,27 +1236,27 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1198,12 +1266,12 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1223,7 +1291,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1238,7 +1306,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1258,7 +1326,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1273,12 +1341,12 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1298,12 +1366,12 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1333,7 +1401,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1363,7 +1431,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1383,12 +1451,12 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="4" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1403,7 +1471,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1413,7 +1481,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="4" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1423,7 +1491,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="4" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1443,37 +1511,37 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1498,7 +1566,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="6" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1513,7 +1581,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1523,7 +1591,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1533,7 +1601,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="5" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1548,7 +1616,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="3" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1558,7 +1626,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1573,17 +1641,17 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="5" t="s">
+      <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="8" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1603,7 +1671,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="5" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1613,7 +1681,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="7" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1623,22 +1691,22 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="4" t="s">
+      <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="5" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1653,42 +1721,42 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="s">
+      <c r="A167" s="4" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="7" t="s">
+      <c r="A168" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="3" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="s">
+      <c r="A172" s="6" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="5" t="s">
+      <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1703,2437 +1771,2448 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="8"/>
+      <c r="A177" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="178">
-      <c r="A178" s="8"/>
+      <c r="A178" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="179">
-      <c r="A179" s="8"/>
+      <c r="A179" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="180">
-      <c r="A180" s="8"/>
+      <c r="A180" s="4" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="181">
-      <c r="A181" s="8"/>
+      <c r="A181" s="2" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="182">
-      <c r="A182" s="8"/>
+      <c r="A182" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="183">
-      <c r="A183" s="8"/>
+      <c r="A183" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="184">
-      <c r="A184" s="8"/>
+      <c r="A184" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="185">
-      <c r="A185" s="8"/>
+      <c r="A185" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="186">
-      <c r="A186" s="8"/>
+      <c r="A186" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="187">
-      <c r="A187" s="8"/>
+      <c r="A187" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" s="8"/>
+      <c r="A188" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" s="8"/>
+      <c r="A189" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="190">
-      <c r="A190" s="8"/>
+      <c r="A190" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="191">
-      <c r="A191" s="8"/>
+      <c r="A191" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="192">
-      <c r="A192" s="8"/>
+      <c r="A192" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="193">
-      <c r="A193" s="8"/>
+      <c r="A193" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="194">
-      <c r="A194" s="8"/>
+      <c r="A194" s="6" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="195">
-      <c r="A195" s="8"/>
+      <c r="A195" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="196">
-      <c r="A196" s="8"/>
+      <c r="A196" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="197">
-      <c r="A197" s="8"/>
+      <c r="A197" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="198">
-      <c r="A198" s="8"/>
+      <c r="A198" s="2" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="199">
-      <c r="A199" s="8"/>
+      <c r="A199" s="4"/>
     </row>
     <row r="200">
-      <c r="A200" s="8"/>
+      <c r="A200" s="4"/>
     </row>
     <row r="201">
-      <c r="A201" s="8"/>
+      <c r="A201" s="4"/>
     </row>
     <row r="202">
-      <c r="A202" s="8"/>
+      <c r="A202" s="4"/>
     </row>
     <row r="203">
-      <c r="A203" s="8"/>
+      <c r="A203" s="4"/>
     </row>
     <row r="204">
-      <c r="A204" s="8"/>
+      <c r="A204" s="4"/>
     </row>
     <row r="205">
-      <c r="A205" s="8"/>
+      <c r="A205" s="4"/>
     </row>
     <row r="206">
-      <c r="A206" s="8"/>
+      <c r="A206" s="4"/>
     </row>
     <row r="207">
-      <c r="A207" s="8"/>
+      <c r="A207" s="4"/>
     </row>
     <row r="208">
-      <c r="A208" s="8"/>
+      <c r="A208" s="4"/>
     </row>
     <row r="209">
-      <c r="A209" s="8"/>
+      <c r="A209" s="4"/>
     </row>
     <row r="210">
-      <c r="A210" s="8"/>
+      <c r="A210" s="4"/>
     </row>
     <row r="211">
-      <c r="A211" s="8"/>
+      <c r="A211" s="4"/>
     </row>
     <row r="212">
-      <c r="A212" s="8"/>
+      <c r="A212" s="4"/>
     </row>
     <row r="213">
-      <c r="A213" s="8"/>
+      <c r="A213" s="4"/>
     </row>
     <row r="214">
-      <c r="A214" s="8"/>
+      <c r="A214" s="4"/>
     </row>
     <row r="215">
-      <c r="A215" s="8"/>
+      <c r="A215" s="4"/>
     </row>
     <row r="216">
-      <c r="A216" s="8"/>
+      <c r="A216" s="4"/>
     </row>
     <row r="217">
-      <c r="A217" s="8"/>
+      <c r="A217" s="4"/>
     </row>
     <row r="218">
-      <c r="A218" s="8"/>
+      <c r="A218" s="4"/>
     </row>
     <row r="219">
-      <c r="A219" s="8"/>
+      <c r="A219" s="4"/>
     </row>
     <row r="220">
-      <c r="A220" s="8"/>
+      <c r="A220" s="4"/>
     </row>
     <row r="221">
-      <c r="A221" s="8"/>
+      <c r="A221" s="4"/>
     </row>
     <row r="222">
-      <c r="A222" s="8"/>
+      <c r="A222" s="4"/>
     </row>
     <row r="223">
-      <c r="A223" s="8"/>
+      <c r="A223" s="4"/>
     </row>
     <row r="224">
-      <c r="A224" s="8"/>
+      <c r="A224" s="4"/>
     </row>
     <row r="225">
-      <c r="A225" s="8"/>
+      <c r="A225" s="4"/>
     </row>
     <row r="226">
-      <c r="A226" s="8"/>
+      <c r="A226" s="4"/>
     </row>
     <row r="227">
-      <c r="A227" s="8"/>
+      <c r="A227" s="4"/>
     </row>
     <row r="228">
-      <c r="A228" s="8"/>
+      <c r="A228" s="4"/>
     </row>
     <row r="229">
-      <c r="A229" s="8"/>
+      <c r="A229" s="4"/>
     </row>
     <row r="230">
-      <c r="A230" s="8"/>
+      <c r="A230" s="4"/>
     </row>
     <row r="231">
-      <c r="A231" s="8"/>
+      <c r="A231" s="4"/>
     </row>
     <row r="232">
-      <c r="A232" s="8"/>
+      <c r="A232" s="4"/>
     </row>
     <row r="233">
-      <c r="A233" s="8"/>
+      <c r="A233" s="4"/>
     </row>
     <row r="234">
-      <c r="A234" s="8"/>
+      <c r="A234" s="4"/>
     </row>
     <row r="235">
-      <c r="A235" s="8"/>
+      <c r="A235" s="4"/>
     </row>
     <row r="236">
-      <c r="A236" s="8"/>
+      <c r="A236" s="4"/>
     </row>
     <row r="237">
-      <c r="A237" s="8"/>
+      <c r="A237" s="4"/>
     </row>
     <row r="238">
-      <c r="A238" s="8"/>
+      <c r="A238" s="4"/>
     </row>
     <row r="239">
-      <c r="A239" s="8"/>
+      <c r="A239" s="4"/>
     </row>
     <row r="240">
-      <c r="A240" s="8"/>
+      <c r="A240" s="4"/>
     </row>
     <row r="241">
-      <c r="A241" s="8"/>
+      <c r="A241" s="4"/>
     </row>
     <row r="242">
-      <c r="A242" s="8"/>
+      <c r="A242" s="4"/>
     </row>
     <row r="243">
-      <c r="A243" s="8"/>
+      <c r="A243" s="4"/>
     </row>
     <row r="244">
-      <c r="A244" s="8"/>
+      <c r="A244" s="4"/>
     </row>
     <row r="245">
-      <c r="A245" s="8"/>
+      <c r="A245" s="4"/>
     </row>
     <row r="246">
-      <c r="A246" s="8"/>
+      <c r="A246" s="4"/>
     </row>
     <row r="247">
-      <c r="A247" s="8"/>
+      <c r="A247" s="4"/>
     </row>
     <row r="248">
-      <c r="A248" s="8"/>
+      <c r="A248" s="4"/>
     </row>
     <row r="249">
-      <c r="A249" s="8"/>
+      <c r="A249" s="4"/>
     </row>
     <row r="250">
-      <c r="A250" s="8"/>
+      <c r="A250" s="4"/>
     </row>
     <row r="251">
-      <c r="A251" s="8"/>
+      <c r="A251" s="4"/>
     </row>
     <row r="252">
-      <c r="A252" s="8"/>
+      <c r="A252" s="4"/>
     </row>
     <row r="253">
-      <c r="A253" s="8"/>
+      <c r="A253" s="4"/>
     </row>
     <row r="254">
-      <c r="A254" s="8"/>
+      <c r="A254" s="4"/>
     </row>
     <row r="255">
-      <c r="A255" s="8"/>
+      <c r="A255" s="4"/>
     </row>
     <row r="256">
-      <c r="A256" s="8"/>
+      <c r="A256" s="4"/>
     </row>
     <row r="257">
-      <c r="A257" s="8"/>
+      <c r="A257" s="4"/>
     </row>
     <row r="258">
-      <c r="A258" s="8"/>
+      <c r="A258" s="4"/>
     </row>
     <row r="259">
-      <c r="A259" s="8"/>
+      <c r="A259" s="4"/>
     </row>
     <row r="260">
-      <c r="A260" s="8"/>
+      <c r="A260" s="4"/>
     </row>
     <row r="261">
-      <c r="A261" s="8"/>
+      <c r="A261" s="4"/>
     </row>
     <row r="262">
-      <c r="A262" s="8"/>
+      <c r="A262" s="4"/>
     </row>
     <row r="263">
-      <c r="A263" s="8"/>
+      <c r="A263" s="4"/>
     </row>
     <row r="264">
-      <c r="A264" s="8"/>
+      <c r="A264" s="4"/>
     </row>
     <row r="265">
-      <c r="A265" s="8"/>
+      <c r="A265" s="4"/>
     </row>
     <row r="266">
-      <c r="A266" s="8"/>
+      <c r="A266" s="4"/>
     </row>
     <row r="267">
-      <c r="A267" s="8"/>
+      <c r="A267" s="4"/>
     </row>
     <row r="268">
-      <c r="A268" s="8"/>
+      <c r="A268" s="4"/>
     </row>
     <row r="269">
-      <c r="A269" s="8"/>
+      <c r="A269" s="4"/>
     </row>
     <row r="270">
-      <c r="A270" s="8"/>
+      <c r="A270" s="4"/>
     </row>
     <row r="271">
-      <c r="A271" s="8"/>
+      <c r="A271" s="4"/>
     </row>
     <row r="272">
-      <c r="A272" s="8"/>
+      <c r="A272" s="4"/>
     </row>
     <row r="273">
-      <c r="A273" s="8"/>
+      <c r="A273" s="4"/>
     </row>
     <row r="274">
-      <c r="A274" s="8"/>
+      <c r="A274" s="4"/>
     </row>
     <row r="275">
-      <c r="A275" s="8"/>
+      <c r="A275" s="4"/>
     </row>
     <row r="276">
-      <c r="A276" s="8"/>
+      <c r="A276" s="4"/>
     </row>
     <row r="277">
-      <c r="A277" s="8"/>
+      <c r="A277" s="4"/>
     </row>
     <row r="278">
-      <c r="A278" s="8"/>
+      <c r="A278" s="4"/>
     </row>
     <row r="279">
-      <c r="A279" s="8"/>
+      <c r="A279" s="4"/>
     </row>
     <row r="280">
-      <c r="A280" s="8"/>
+      <c r="A280" s="4"/>
     </row>
     <row r="281">
-      <c r="A281" s="8"/>
+      <c r="A281" s="4"/>
     </row>
     <row r="282">
-      <c r="A282" s="8"/>
+      <c r="A282" s="4"/>
     </row>
     <row r="283">
-      <c r="A283" s="8"/>
+      <c r="A283" s="4"/>
     </row>
     <row r="284">
-      <c r="A284" s="8"/>
+      <c r="A284" s="4"/>
     </row>
     <row r="285">
-      <c r="A285" s="8"/>
+      <c r="A285" s="4"/>
     </row>
     <row r="286">
-      <c r="A286" s="8"/>
+      <c r="A286" s="4"/>
     </row>
     <row r="287">
-      <c r="A287" s="8"/>
+      <c r="A287" s="4"/>
     </row>
     <row r="288">
-      <c r="A288" s="8"/>
+      <c r="A288" s="4"/>
     </row>
     <row r="289">
-      <c r="A289" s="8"/>
+      <c r="A289" s="4"/>
     </row>
     <row r="290">
-      <c r="A290" s="8"/>
+      <c r="A290" s="4"/>
     </row>
     <row r="291">
-      <c r="A291" s="8"/>
+      <c r="A291" s="4"/>
     </row>
     <row r="292">
-      <c r="A292" s="8"/>
+      <c r="A292" s="4"/>
     </row>
     <row r="293">
-      <c r="A293" s="8"/>
+      <c r="A293" s="4"/>
     </row>
     <row r="294">
-      <c r="A294" s="8"/>
+      <c r="A294" s="4"/>
     </row>
     <row r="295">
-      <c r="A295" s="8"/>
+      <c r="A295" s="4"/>
     </row>
     <row r="296">
-      <c r="A296" s="8"/>
+      <c r="A296" s="4"/>
     </row>
     <row r="297">
-      <c r="A297" s="8"/>
+      <c r="A297" s="4"/>
     </row>
     <row r="298">
-      <c r="A298" s="8"/>
+      <c r="A298" s="4"/>
     </row>
     <row r="299">
-      <c r="A299" s="8"/>
+      <c r="A299" s="4"/>
     </row>
     <row r="300">
-      <c r="A300" s="8"/>
+      <c r="A300" s="4"/>
     </row>
     <row r="301">
-      <c r="A301" s="8"/>
+      <c r="A301" s="4"/>
     </row>
     <row r="302">
-      <c r="A302" s="8"/>
+      <c r="A302" s="4"/>
     </row>
     <row r="303">
-      <c r="A303" s="8"/>
+      <c r="A303" s="4"/>
     </row>
     <row r="304">
-      <c r="A304" s="8"/>
+      <c r="A304" s="4"/>
     </row>
     <row r="305">
-      <c r="A305" s="8"/>
+      <c r="A305" s="4"/>
     </row>
     <row r="306">
-      <c r="A306" s="8"/>
+      <c r="A306" s="4"/>
     </row>
     <row r="307">
-      <c r="A307" s="8"/>
+      <c r="A307" s="4"/>
     </row>
     <row r="308">
-      <c r="A308" s="8"/>
+      <c r="A308" s="4"/>
     </row>
     <row r="309">
-      <c r="A309" s="8"/>
+      <c r="A309" s="4"/>
     </row>
     <row r="310">
-      <c r="A310" s="8"/>
+      <c r="A310" s="4"/>
     </row>
     <row r="311">
-      <c r="A311" s="8"/>
+      <c r="A311" s="4"/>
     </row>
     <row r="312">
-      <c r="A312" s="8"/>
+      <c r="A312" s="4"/>
     </row>
     <row r="313">
-      <c r="A313" s="8"/>
+      <c r="A313" s="4"/>
     </row>
     <row r="314">
-      <c r="A314" s="8"/>
+      <c r="A314" s="4"/>
     </row>
     <row r="315">
-      <c r="A315" s="8"/>
+      <c r="A315" s="4"/>
     </row>
     <row r="316">
-      <c r="A316" s="8"/>
+      <c r="A316" s="4"/>
     </row>
     <row r="317">
-      <c r="A317" s="8"/>
+      <c r="A317" s="4"/>
     </row>
     <row r="318">
-      <c r="A318" s="8"/>
+      <c r="A318" s="4"/>
     </row>
     <row r="319">
-      <c r="A319" s="8"/>
+      <c r="A319" s="4"/>
     </row>
     <row r="320">
-      <c r="A320" s="8"/>
+      <c r="A320" s="4"/>
     </row>
     <row r="321">
-      <c r="A321" s="8"/>
+      <c r="A321" s="4"/>
     </row>
     <row r="322">
-      <c r="A322" s="8"/>
+      <c r="A322" s="4"/>
     </row>
     <row r="323">
-      <c r="A323" s="8"/>
+      <c r="A323" s="4"/>
     </row>
     <row r="324">
-      <c r="A324" s="8"/>
+      <c r="A324" s="4"/>
     </row>
     <row r="325">
-      <c r="A325" s="8"/>
+      <c r="A325" s="4"/>
     </row>
     <row r="326">
-      <c r="A326" s="8"/>
+      <c r="A326" s="4"/>
     </row>
     <row r="327">
-      <c r="A327" s="8"/>
+      <c r="A327" s="4"/>
     </row>
     <row r="328">
-      <c r="A328" s="8"/>
+      <c r="A328" s="4"/>
     </row>
     <row r="329">
-      <c r="A329" s="8"/>
+      <c r="A329" s="4"/>
     </row>
     <row r="330">
-      <c r="A330" s="8"/>
+      <c r="A330" s="4"/>
     </row>
     <row r="331">
-      <c r="A331" s="8"/>
+      <c r="A331" s="4"/>
     </row>
     <row r="332">
-      <c r="A332" s="8"/>
+      <c r="A332" s="4"/>
     </row>
     <row r="333">
-      <c r="A333" s="8"/>
+      <c r="A333" s="4"/>
     </row>
     <row r="334">
-      <c r="A334" s="8"/>
+      <c r="A334" s="4"/>
     </row>
     <row r="335">
-      <c r="A335" s="8"/>
+      <c r="A335" s="4"/>
     </row>
     <row r="336">
-      <c r="A336" s="8"/>
+      <c r="A336" s="4"/>
     </row>
     <row r="337">
-      <c r="A337" s="8"/>
+      <c r="A337" s="4"/>
     </row>
     <row r="338">
-      <c r="A338" s="8"/>
+      <c r="A338" s="4"/>
     </row>
     <row r="339">
-      <c r="A339" s="8"/>
+      <c r="A339" s="4"/>
     </row>
     <row r="340">
-      <c r="A340" s="8"/>
+      <c r="A340" s="4"/>
     </row>
     <row r="341">
-      <c r="A341" s="8"/>
+      <c r="A341" s="4"/>
     </row>
     <row r="342">
-      <c r="A342" s="8"/>
+      <c r="A342" s="4"/>
     </row>
     <row r="343">
-      <c r="A343" s="8"/>
+      <c r="A343" s="4"/>
     </row>
     <row r="344">
-      <c r="A344" s="8"/>
+      <c r="A344" s="4"/>
     </row>
     <row r="345">
-      <c r="A345" s="8"/>
+      <c r="A345" s="4"/>
     </row>
     <row r="346">
-      <c r="A346" s="8"/>
+      <c r="A346" s="4"/>
     </row>
     <row r="347">
-      <c r="A347" s="8"/>
+      <c r="A347" s="4"/>
     </row>
     <row r="348">
-      <c r="A348" s="8"/>
+      <c r="A348" s="4"/>
     </row>
     <row r="349">
-      <c r="A349" s="8"/>
+      <c r="A349" s="4"/>
     </row>
     <row r="350">
-      <c r="A350" s="8"/>
+      <c r="A350" s="4"/>
     </row>
     <row r="351">
-      <c r="A351" s="8"/>
+      <c r="A351" s="4"/>
     </row>
     <row r="352">
-      <c r="A352" s="8"/>
+      <c r="A352" s="4"/>
     </row>
     <row r="353">
-      <c r="A353" s="8"/>
+      <c r="A353" s="4"/>
     </row>
     <row r="354">
-      <c r="A354" s="8"/>
+      <c r="A354" s="4"/>
     </row>
     <row r="355">
-      <c r="A355" s="8"/>
+      <c r="A355" s="4"/>
     </row>
     <row r="356">
-      <c r="A356" s="8"/>
+      <c r="A356" s="4"/>
     </row>
     <row r="357">
-      <c r="A357" s="8"/>
+      <c r="A357" s="4"/>
     </row>
     <row r="358">
-      <c r="A358" s="8"/>
+      <c r="A358" s="4"/>
     </row>
     <row r="359">
-      <c r="A359" s="8"/>
+      <c r="A359" s="4"/>
     </row>
     <row r="360">
-      <c r="A360" s="8"/>
+      <c r="A360" s="4"/>
     </row>
     <row r="361">
-      <c r="A361" s="8"/>
+      <c r="A361" s="4"/>
     </row>
     <row r="362">
-      <c r="A362" s="8"/>
+      <c r="A362" s="4"/>
     </row>
     <row r="363">
-      <c r="A363" s="8"/>
+      <c r="A363" s="4"/>
     </row>
     <row r="364">
-      <c r="A364" s="8"/>
+      <c r="A364" s="4"/>
     </row>
     <row r="365">
-      <c r="A365" s="8"/>
+      <c r="A365" s="4"/>
     </row>
     <row r="366">
-      <c r="A366" s="8"/>
+      <c r="A366" s="4"/>
     </row>
     <row r="367">
-      <c r="A367" s="8"/>
+      <c r="A367" s="4"/>
     </row>
     <row r="368">
-      <c r="A368" s="8"/>
+      <c r="A368" s="4"/>
     </row>
     <row r="369">
-      <c r="A369" s="8"/>
+      <c r="A369" s="4"/>
     </row>
     <row r="370">
-      <c r="A370" s="8"/>
+      <c r="A370" s="4"/>
     </row>
     <row r="371">
-      <c r="A371" s="8"/>
+      <c r="A371" s="4"/>
     </row>
     <row r="372">
-      <c r="A372" s="8"/>
+      <c r="A372" s="4"/>
     </row>
     <row r="373">
-      <c r="A373" s="8"/>
+      <c r="A373" s="4"/>
     </row>
     <row r="374">
-      <c r="A374" s="8"/>
+      <c r="A374" s="4"/>
     </row>
     <row r="375">
-      <c r="A375" s="8"/>
+      <c r="A375" s="4"/>
     </row>
     <row r="376">
-      <c r="A376" s="8"/>
+      <c r="A376" s="4"/>
     </row>
     <row r="377">
-      <c r="A377" s="8"/>
+      <c r="A377" s="4"/>
     </row>
     <row r="378">
-      <c r="A378" s="8"/>
+      <c r="A378" s="4"/>
     </row>
     <row r="379">
-      <c r="A379" s="8"/>
+      <c r="A379" s="4"/>
     </row>
     <row r="380">
-      <c r="A380" s="8"/>
+      <c r="A380" s="4"/>
     </row>
     <row r="381">
-      <c r="A381" s="8"/>
+      <c r="A381" s="4"/>
     </row>
     <row r="382">
-      <c r="A382" s="8"/>
+      <c r="A382" s="4"/>
     </row>
     <row r="383">
-      <c r="A383" s="8"/>
+      <c r="A383" s="4"/>
     </row>
     <row r="384">
-      <c r="A384" s="8"/>
+      <c r="A384" s="4"/>
     </row>
     <row r="385">
-      <c r="A385" s="8"/>
+      <c r="A385" s="4"/>
     </row>
     <row r="386">
-      <c r="A386" s="8"/>
+      <c r="A386" s="4"/>
     </row>
     <row r="387">
-      <c r="A387" s="8"/>
+      <c r="A387" s="4"/>
     </row>
     <row r="388">
-      <c r="A388" s="8"/>
+      <c r="A388" s="4"/>
     </row>
     <row r="389">
-      <c r="A389" s="8"/>
+      <c r="A389" s="4"/>
     </row>
     <row r="390">
-      <c r="A390" s="8"/>
+      <c r="A390" s="4"/>
     </row>
     <row r="391">
-      <c r="A391" s="8"/>
+      <c r="A391" s="4"/>
     </row>
     <row r="392">
-      <c r="A392" s="8"/>
+      <c r="A392" s="4"/>
     </row>
     <row r="393">
-      <c r="A393" s="8"/>
+      <c r="A393" s="4"/>
     </row>
     <row r="394">
-      <c r="A394" s="8"/>
+      <c r="A394" s="4"/>
     </row>
     <row r="395">
-      <c r="A395" s="8"/>
+      <c r="A395" s="4"/>
     </row>
     <row r="396">
-      <c r="A396" s="8"/>
+      <c r="A396" s="4"/>
     </row>
     <row r="397">
-      <c r="A397" s="8"/>
+      <c r="A397" s="4"/>
     </row>
     <row r="398">
-      <c r="A398" s="8"/>
+      <c r="A398" s="4"/>
     </row>
     <row r="399">
-      <c r="A399" s="8"/>
+      <c r="A399" s="4"/>
     </row>
     <row r="400">
-      <c r="A400" s="8"/>
+      <c r="A400" s="4"/>
     </row>
     <row r="401">
-      <c r="A401" s="8"/>
+      <c r="A401" s="4"/>
     </row>
     <row r="402">
-      <c r="A402" s="8"/>
+      <c r="A402" s="4"/>
     </row>
     <row r="403">
-      <c r="A403" s="8"/>
+      <c r="A403" s="4"/>
     </row>
     <row r="404">
-      <c r="A404" s="8"/>
+      <c r="A404" s="4"/>
     </row>
     <row r="405">
-      <c r="A405" s="8"/>
+      <c r="A405" s="4"/>
     </row>
     <row r="406">
-      <c r="A406" s="8"/>
+      <c r="A406" s="4"/>
     </row>
     <row r="407">
-      <c r="A407" s="8"/>
+      <c r="A407" s="4"/>
     </row>
     <row r="408">
-      <c r="A408" s="8"/>
+      <c r="A408" s="4"/>
     </row>
     <row r="409">
-      <c r="A409" s="8"/>
+      <c r="A409" s="4"/>
     </row>
     <row r="410">
-      <c r="A410" s="8"/>
+      <c r="A410" s="4"/>
     </row>
     <row r="411">
-      <c r="A411" s="8"/>
+      <c r="A411" s="4"/>
     </row>
     <row r="412">
-      <c r="A412" s="8"/>
+      <c r="A412" s="4"/>
     </row>
     <row r="413">
-      <c r="A413" s="8"/>
+      <c r="A413" s="4"/>
     </row>
     <row r="414">
-      <c r="A414" s="8"/>
+      <c r="A414" s="4"/>
     </row>
     <row r="415">
-      <c r="A415" s="8"/>
+      <c r="A415" s="4"/>
     </row>
     <row r="416">
-      <c r="A416" s="8"/>
+      <c r="A416" s="4"/>
     </row>
     <row r="417">
-      <c r="A417" s="8"/>
+      <c r="A417" s="4"/>
     </row>
     <row r="418">
-      <c r="A418" s="8"/>
+      <c r="A418" s="4"/>
     </row>
     <row r="419">
-      <c r="A419" s="8"/>
+      <c r="A419" s="4"/>
     </row>
     <row r="420">
-      <c r="A420" s="8"/>
+      <c r="A420" s="4"/>
     </row>
     <row r="421">
-      <c r="A421" s="8"/>
+      <c r="A421" s="4"/>
     </row>
     <row r="422">
-      <c r="A422" s="8"/>
+      <c r="A422" s="4"/>
     </row>
     <row r="423">
-      <c r="A423" s="8"/>
+      <c r="A423" s="4"/>
     </row>
     <row r="424">
-      <c r="A424" s="8"/>
+      <c r="A424" s="4"/>
     </row>
     <row r="425">
-      <c r="A425" s="8"/>
+      <c r="A425" s="4"/>
     </row>
     <row r="426">
-      <c r="A426" s="8"/>
+      <c r="A426" s="4"/>
     </row>
     <row r="427">
-      <c r="A427" s="8"/>
+      <c r="A427" s="4"/>
     </row>
     <row r="428">
-      <c r="A428" s="8"/>
+      <c r="A428" s="4"/>
     </row>
     <row r="429">
-      <c r="A429" s="8"/>
+      <c r="A429" s="4"/>
     </row>
     <row r="430">
-      <c r="A430" s="8"/>
+      <c r="A430" s="4"/>
     </row>
     <row r="431">
-      <c r="A431" s="8"/>
+      <c r="A431" s="4"/>
     </row>
     <row r="432">
-      <c r="A432" s="8"/>
+      <c r="A432" s="4"/>
     </row>
     <row r="433">
-      <c r="A433" s="8"/>
+      <c r="A433" s="4"/>
     </row>
     <row r="434">
-      <c r="A434" s="8"/>
+      <c r="A434" s="4"/>
     </row>
     <row r="435">
-      <c r="A435" s="8"/>
+      <c r="A435" s="4"/>
     </row>
     <row r="436">
-      <c r="A436" s="8"/>
+      <c r="A436" s="4"/>
     </row>
     <row r="437">
-      <c r="A437" s="8"/>
+      <c r="A437" s="4"/>
     </row>
     <row r="438">
-      <c r="A438" s="8"/>
+      <c r="A438" s="4"/>
     </row>
     <row r="439">
-      <c r="A439" s="8"/>
+      <c r="A439" s="4"/>
     </row>
     <row r="440">
-      <c r="A440" s="8"/>
+      <c r="A440" s="4"/>
     </row>
     <row r="441">
-      <c r="A441" s="8"/>
+      <c r="A441" s="4"/>
     </row>
     <row r="442">
-      <c r="A442" s="8"/>
+      <c r="A442" s="4"/>
     </row>
     <row r="443">
-      <c r="A443" s="8"/>
+      <c r="A443" s="4"/>
     </row>
     <row r="444">
-      <c r="A444" s="8"/>
+      <c r="A444" s="4"/>
     </row>
     <row r="445">
-      <c r="A445" s="8"/>
+      <c r="A445" s="4"/>
     </row>
     <row r="446">
-      <c r="A446" s="8"/>
+      <c r="A446" s="4"/>
     </row>
     <row r="447">
-      <c r="A447" s="8"/>
+      <c r="A447" s="4"/>
     </row>
     <row r="448">
-      <c r="A448" s="8"/>
+      <c r="A448" s="4"/>
     </row>
     <row r="449">
-      <c r="A449" s="8"/>
+      <c r="A449" s="4"/>
     </row>
     <row r="450">
-      <c r="A450" s="8"/>
+      <c r="A450" s="4"/>
     </row>
     <row r="451">
-      <c r="A451" s="8"/>
+      <c r="A451" s="4"/>
     </row>
     <row r="452">
-      <c r="A452" s="8"/>
+      <c r="A452" s="4"/>
     </row>
     <row r="453">
-      <c r="A453" s="8"/>
+      <c r="A453" s="4"/>
     </row>
     <row r="454">
-      <c r="A454" s="8"/>
+      <c r="A454" s="4"/>
     </row>
     <row r="455">
-      <c r="A455" s="8"/>
+      <c r="A455" s="4"/>
     </row>
     <row r="456">
-      <c r="A456" s="8"/>
+      <c r="A456" s="4"/>
     </row>
     <row r="457">
-      <c r="A457" s="8"/>
+      <c r="A457" s="4"/>
     </row>
     <row r="458">
-      <c r="A458" s="8"/>
+      <c r="A458" s="4"/>
     </row>
     <row r="459">
-      <c r="A459" s="8"/>
+      <c r="A459" s="4"/>
     </row>
     <row r="460">
-      <c r="A460" s="8"/>
+      <c r="A460" s="4"/>
     </row>
     <row r="461">
-      <c r="A461" s="8"/>
+      <c r="A461" s="4"/>
     </row>
     <row r="462">
-      <c r="A462" s="8"/>
+      <c r="A462" s="4"/>
     </row>
     <row r="463">
-      <c r="A463" s="8"/>
+      <c r="A463" s="4"/>
     </row>
     <row r="464">
-      <c r="A464" s="8"/>
+      <c r="A464" s="4"/>
     </row>
     <row r="465">
-      <c r="A465" s="8"/>
+      <c r="A465" s="4"/>
     </row>
     <row r="466">
-      <c r="A466" s="8"/>
+      <c r="A466" s="4"/>
     </row>
     <row r="467">
-      <c r="A467" s="8"/>
+      <c r="A467" s="4"/>
     </row>
     <row r="468">
-      <c r="A468" s="8"/>
+      <c r="A468" s="4"/>
     </row>
     <row r="469">
-      <c r="A469" s="8"/>
+      <c r="A469" s="4"/>
     </row>
     <row r="470">
-      <c r="A470" s="8"/>
+      <c r="A470" s="4"/>
     </row>
     <row r="471">
-      <c r="A471" s="8"/>
+      <c r="A471" s="4"/>
     </row>
     <row r="472">
-      <c r="A472" s="8"/>
+      <c r="A472" s="4"/>
     </row>
     <row r="473">
-      <c r="A473" s="8"/>
+      <c r="A473" s="4"/>
     </row>
     <row r="474">
-      <c r="A474" s="8"/>
+      <c r="A474" s="4"/>
     </row>
     <row r="475">
-      <c r="A475" s="8"/>
+      <c r="A475" s="4"/>
     </row>
     <row r="476">
-      <c r="A476" s="8"/>
+      <c r="A476" s="4"/>
     </row>
     <row r="477">
-      <c r="A477" s="8"/>
+      <c r="A477" s="4"/>
     </row>
     <row r="478">
-      <c r="A478" s="8"/>
+      <c r="A478" s="4"/>
     </row>
     <row r="479">
-      <c r="A479" s="8"/>
+      <c r="A479" s="4"/>
     </row>
     <row r="480">
-      <c r="A480" s="8"/>
+      <c r="A480" s="4"/>
     </row>
     <row r="481">
-      <c r="A481" s="8"/>
+      <c r="A481" s="4"/>
     </row>
     <row r="482">
-      <c r="A482" s="8"/>
+      <c r="A482" s="4"/>
     </row>
     <row r="483">
-      <c r="A483" s="8"/>
+      <c r="A483" s="4"/>
     </row>
     <row r="484">
-      <c r="A484" s="8"/>
+      <c r="A484" s="4"/>
     </row>
     <row r="485">
-      <c r="A485" s="8"/>
+      <c r="A485" s="4"/>
     </row>
     <row r="486">
-      <c r="A486" s="8"/>
+      <c r="A486" s="4"/>
     </row>
     <row r="487">
-      <c r="A487" s="8"/>
+      <c r="A487" s="4"/>
     </row>
     <row r="488">
-      <c r="A488" s="8"/>
+      <c r="A488" s="4"/>
     </row>
     <row r="489">
-      <c r="A489" s="8"/>
+      <c r="A489" s="4"/>
     </row>
     <row r="490">
-      <c r="A490" s="8"/>
+      <c r="A490" s="4"/>
     </row>
     <row r="491">
-      <c r="A491" s="8"/>
+      <c r="A491" s="4"/>
     </row>
     <row r="492">
-      <c r="A492" s="8"/>
+      <c r="A492" s="4"/>
     </row>
     <row r="493">
-      <c r="A493" s="8"/>
+      <c r="A493" s="4"/>
     </row>
     <row r="494">
-      <c r="A494" s="8"/>
+      <c r="A494" s="4"/>
     </row>
     <row r="495">
-      <c r="A495" s="8"/>
+      <c r="A495" s="4"/>
     </row>
     <row r="496">
-      <c r="A496" s="8"/>
+      <c r="A496" s="4"/>
     </row>
     <row r="497">
-      <c r="A497" s="8"/>
+      <c r="A497" s="4"/>
     </row>
     <row r="498">
-      <c r="A498" s="8"/>
+      <c r="A498" s="4"/>
     </row>
     <row r="499">
-      <c r="A499" s="8"/>
+      <c r="A499" s="4"/>
     </row>
     <row r="500">
-      <c r="A500" s="8"/>
+      <c r="A500" s="4"/>
     </row>
     <row r="501">
-      <c r="A501" s="8"/>
+      <c r="A501" s="4"/>
     </row>
     <row r="502">
-      <c r="A502" s="8"/>
+      <c r="A502" s="4"/>
     </row>
     <row r="503">
-      <c r="A503" s="8"/>
+      <c r="A503" s="4"/>
     </row>
     <row r="504">
-      <c r="A504" s="8"/>
+      <c r="A504" s="4"/>
     </row>
     <row r="505">
-      <c r="A505" s="8"/>
+      <c r="A505" s="4"/>
     </row>
     <row r="506">
-      <c r="A506" s="8"/>
+      <c r="A506" s="4"/>
     </row>
     <row r="507">
-      <c r="A507" s="8"/>
+      <c r="A507" s="4"/>
     </row>
     <row r="508">
-      <c r="A508" s="8"/>
+      <c r="A508" s="4"/>
     </row>
     <row r="509">
-      <c r="A509" s="8"/>
+      <c r="A509" s="4"/>
     </row>
     <row r="510">
-      <c r="A510" s="8"/>
+      <c r="A510" s="4"/>
     </row>
     <row r="511">
-      <c r="A511" s="8"/>
+      <c r="A511" s="4"/>
     </row>
     <row r="512">
-      <c r="A512" s="8"/>
+      <c r="A512" s="4"/>
     </row>
     <row r="513">
-      <c r="A513" s="8"/>
+      <c r="A513" s="4"/>
     </row>
     <row r="514">
-      <c r="A514" s="8"/>
+      <c r="A514" s="4"/>
     </row>
     <row r="515">
-      <c r="A515" s="8"/>
+      <c r="A515" s="4"/>
     </row>
     <row r="516">
-      <c r="A516" s="8"/>
+      <c r="A516" s="4"/>
     </row>
     <row r="517">
-      <c r="A517" s="8"/>
+      <c r="A517" s="4"/>
     </row>
     <row r="518">
-      <c r="A518" s="8"/>
+      <c r="A518" s="4"/>
     </row>
     <row r="519">
-      <c r="A519" s="8"/>
+      <c r="A519" s="4"/>
     </row>
     <row r="520">
-      <c r="A520" s="8"/>
+      <c r="A520" s="4"/>
     </row>
     <row r="521">
-      <c r="A521" s="8"/>
+      <c r="A521" s="4"/>
     </row>
     <row r="522">
-      <c r="A522" s="8"/>
+      <c r="A522" s="4"/>
     </row>
     <row r="523">
-      <c r="A523" s="8"/>
+      <c r="A523" s="4"/>
     </row>
     <row r="524">
-      <c r="A524" s="8"/>
+      <c r="A524" s="4"/>
     </row>
     <row r="525">
-      <c r="A525" s="8"/>
+      <c r="A525" s="4"/>
     </row>
     <row r="526">
-      <c r="A526" s="8"/>
+      <c r="A526" s="4"/>
     </row>
     <row r="527">
-      <c r="A527" s="8"/>
+      <c r="A527" s="4"/>
     </row>
     <row r="528">
-      <c r="A528" s="8"/>
+      <c r="A528" s="4"/>
     </row>
     <row r="529">
-      <c r="A529" s="8"/>
+      <c r="A529" s="4"/>
     </row>
     <row r="530">
-      <c r="A530" s="8"/>
+      <c r="A530" s="4"/>
     </row>
     <row r="531">
-      <c r="A531" s="8"/>
+      <c r="A531" s="4"/>
     </row>
     <row r="532">
-      <c r="A532" s="8"/>
+      <c r="A532" s="4"/>
     </row>
     <row r="533">
-      <c r="A533" s="8"/>
+      <c r="A533" s="4"/>
     </row>
     <row r="534">
-      <c r="A534" s="8"/>
+      <c r="A534" s="4"/>
     </row>
     <row r="535">
-      <c r="A535" s="8"/>
+      <c r="A535" s="4"/>
     </row>
     <row r="536">
-      <c r="A536" s="8"/>
+      <c r="A536" s="4"/>
     </row>
     <row r="537">
-      <c r="A537" s="8"/>
+      <c r="A537" s="4"/>
     </row>
     <row r="538">
-      <c r="A538" s="8"/>
+      <c r="A538" s="4"/>
     </row>
     <row r="539">
-      <c r="A539" s="8"/>
+      <c r="A539" s="4"/>
     </row>
     <row r="540">
-      <c r="A540" s="8"/>
+      <c r="A540" s="4"/>
     </row>
     <row r="541">
-      <c r="A541" s="8"/>
+      <c r="A541" s="4"/>
     </row>
     <row r="542">
-      <c r="A542" s="8"/>
+      <c r="A542" s="4"/>
     </row>
     <row r="543">
-      <c r="A543" s="8"/>
+      <c r="A543" s="4"/>
     </row>
     <row r="544">
-      <c r="A544" s="8"/>
+      <c r="A544" s="4"/>
     </row>
     <row r="545">
-      <c r="A545" s="8"/>
+      <c r="A545" s="4"/>
     </row>
     <row r="546">
-      <c r="A546" s="8"/>
+      <c r="A546" s="4"/>
     </row>
     <row r="547">
-      <c r="A547" s="8"/>
+      <c r="A547" s="4"/>
     </row>
     <row r="548">
-      <c r="A548" s="8"/>
+      <c r="A548" s="4"/>
     </row>
     <row r="549">
-      <c r="A549" s="8"/>
+      <c r="A549" s="4"/>
     </row>
     <row r="550">
-      <c r="A550" s="8"/>
+      <c r="A550" s="4"/>
     </row>
     <row r="551">
-      <c r="A551" s="8"/>
+      <c r="A551" s="4"/>
     </row>
     <row r="552">
-      <c r="A552" s="8"/>
+      <c r="A552" s="4"/>
     </row>
     <row r="553">
-      <c r="A553" s="8"/>
+      <c r="A553" s="4"/>
     </row>
     <row r="554">
-      <c r="A554" s="8"/>
+      <c r="A554" s="4"/>
     </row>
     <row r="555">
-      <c r="A555" s="8"/>
+      <c r="A555" s="4"/>
     </row>
     <row r="556">
-      <c r="A556" s="8"/>
+      <c r="A556" s="4"/>
     </row>
     <row r="557">
-      <c r="A557" s="8"/>
+      <c r="A557" s="4"/>
     </row>
     <row r="558">
-      <c r="A558" s="8"/>
+      <c r="A558" s="4"/>
     </row>
     <row r="559">
-      <c r="A559" s="8"/>
+      <c r="A559" s="4"/>
     </row>
     <row r="560">
-      <c r="A560" s="8"/>
+      <c r="A560" s="4"/>
     </row>
     <row r="561">
-      <c r="A561" s="8"/>
+      <c r="A561" s="4"/>
     </row>
     <row r="562">
-      <c r="A562" s="8"/>
+      <c r="A562" s="4"/>
     </row>
     <row r="563">
-      <c r="A563" s="8"/>
+      <c r="A563" s="4"/>
     </row>
     <row r="564">
-      <c r="A564" s="8"/>
+      <c r="A564" s="4"/>
     </row>
     <row r="565">
-      <c r="A565" s="8"/>
+      <c r="A565" s="4"/>
     </row>
     <row r="566">
-      <c r="A566" s="8"/>
+      <c r="A566" s="4"/>
     </row>
     <row r="567">
-      <c r="A567" s="8"/>
+      <c r="A567" s="4"/>
     </row>
     <row r="568">
-      <c r="A568" s="8"/>
+      <c r="A568" s="4"/>
     </row>
     <row r="569">
-      <c r="A569" s="8"/>
+      <c r="A569" s="4"/>
     </row>
     <row r="570">
-      <c r="A570" s="8"/>
+      <c r="A570" s="4"/>
     </row>
     <row r="571">
-      <c r="A571" s="8"/>
+      <c r="A571" s="4"/>
     </row>
     <row r="572">
-      <c r="A572" s="8"/>
+      <c r="A572" s="4"/>
     </row>
     <row r="573">
-      <c r="A573" s="8"/>
+      <c r="A573" s="4"/>
     </row>
     <row r="574">
-      <c r="A574" s="8"/>
+      <c r="A574" s="4"/>
     </row>
     <row r="575">
-      <c r="A575" s="8"/>
+      <c r="A575" s="4"/>
     </row>
     <row r="576">
-      <c r="A576" s="8"/>
+      <c r="A576" s="4"/>
     </row>
     <row r="577">
-      <c r="A577" s="8"/>
+      <c r="A577" s="4"/>
     </row>
     <row r="578">
-      <c r="A578" s="8"/>
+      <c r="A578" s="4"/>
     </row>
     <row r="579">
-      <c r="A579" s="8"/>
+      <c r="A579" s="4"/>
     </row>
     <row r="580">
-      <c r="A580" s="8"/>
+      <c r="A580" s="4"/>
     </row>
     <row r="581">
-      <c r="A581" s="8"/>
+      <c r="A581" s="4"/>
     </row>
     <row r="582">
-      <c r="A582" s="8"/>
+      <c r="A582" s="4"/>
     </row>
     <row r="583">
-      <c r="A583" s="8"/>
+      <c r="A583" s="4"/>
     </row>
     <row r="584">
-      <c r="A584" s="8"/>
+      <c r="A584" s="4"/>
     </row>
     <row r="585">
-      <c r="A585" s="8"/>
+      <c r="A585" s="4"/>
     </row>
     <row r="586">
-      <c r="A586" s="8"/>
+      <c r="A586" s="4"/>
     </row>
     <row r="587">
-      <c r="A587" s="8"/>
+      <c r="A587" s="4"/>
     </row>
     <row r="588">
-      <c r="A588" s="8"/>
+      <c r="A588" s="4"/>
     </row>
     <row r="589">
-      <c r="A589" s="8"/>
+      <c r="A589" s="4"/>
     </row>
     <row r="590">
-      <c r="A590" s="8"/>
+      <c r="A590" s="4"/>
     </row>
     <row r="591">
-      <c r="A591" s="8"/>
+      <c r="A591" s="4"/>
     </row>
     <row r="592">
-      <c r="A592" s="8"/>
+      <c r="A592" s="4"/>
     </row>
     <row r="593">
-      <c r="A593" s="8"/>
+      <c r="A593" s="4"/>
     </row>
     <row r="594">
-      <c r="A594" s="8"/>
+      <c r="A594" s="4"/>
     </row>
     <row r="595">
-      <c r="A595" s="8"/>
+      <c r="A595" s="4"/>
     </row>
     <row r="596">
-      <c r="A596" s="8"/>
+      <c r="A596" s="4"/>
     </row>
     <row r="597">
-      <c r="A597" s="8"/>
+      <c r="A597" s="4"/>
     </row>
     <row r="598">
-      <c r="A598" s="8"/>
+      <c r="A598" s="4"/>
     </row>
     <row r="599">
-      <c r="A599" s="8"/>
+      <c r="A599" s="4"/>
     </row>
     <row r="600">
-      <c r="A600" s="8"/>
+      <c r="A600" s="4"/>
     </row>
     <row r="601">
-      <c r="A601" s="8"/>
+      <c r="A601" s="4"/>
     </row>
     <row r="602">
-      <c r="A602" s="8"/>
+      <c r="A602" s="4"/>
     </row>
     <row r="603">
-      <c r="A603" s="8"/>
+      <c r="A603" s="4"/>
     </row>
     <row r="604">
-      <c r="A604" s="8"/>
+      <c r="A604" s="4"/>
     </row>
     <row r="605">
-      <c r="A605" s="8"/>
+      <c r="A605" s="4"/>
     </row>
     <row r="606">
-      <c r="A606" s="8"/>
+      <c r="A606" s="4"/>
     </row>
     <row r="607">
-      <c r="A607" s="8"/>
+      <c r="A607" s="4"/>
     </row>
     <row r="608">
-      <c r="A608" s="8"/>
+      <c r="A608" s="4"/>
     </row>
     <row r="609">
-      <c r="A609" s="8"/>
+      <c r="A609" s="4"/>
     </row>
     <row r="610">
-      <c r="A610" s="8"/>
+      <c r="A610" s="4"/>
     </row>
     <row r="611">
-      <c r="A611" s="8"/>
+      <c r="A611" s="4"/>
     </row>
     <row r="612">
-      <c r="A612" s="8"/>
+      <c r="A612" s="4"/>
     </row>
     <row r="613">
-      <c r="A613" s="8"/>
+      <c r="A613" s="4"/>
     </row>
     <row r="614">
-      <c r="A614" s="8"/>
+      <c r="A614" s="4"/>
     </row>
     <row r="615">
-      <c r="A615" s="8"/>
+      <c r="A615" s="4"/>
     </row>
     <row r="616">
-      <c r="A616" s="8"/>
+      <c r="A616" s="4"/>
     </row>
     <row r="617">
-      <c r="A617" s="8"/>
+      <c r="A617" s="4"/>
     </row>
     <row r="618">
-      <c r="A618" s="8"/>
+      <c r="A618" s="4"/>
     </row>
     <row r="619">
-      <c r="A619" s="8"/>
+      <c r="A619" s="4"/>
     </row>
     <row r="620">
-      <c r="A620" s="8"/>
+      <c r="A620" s="4"/>
     </row>
     <row r="621">
-      <c r="A621" s="8"/>
+      <c r="A621" s="4"/>
     </row>
     <row r="622">
-      <c r="A622" s="8"/>
+      <c r="A622" s="4"/>
     </row>
     <row r="623">
-      <c r="A623" s="8"/>
+      <c r="A623" s="4"/>
     </row>
     <row r="624">
-      <c r="A624" s="8"/>
+      <c r="A624" s="4"/>
     </row>
     <row r="625">
-      <c r="A625" s="8"/>
+      <c r="A625" s="4"/>
     </row>
     <row r="626">
-      <c r="A626" s="8"/>
+      <c r="A626" s="4"/>
     </row>
     <row r="627">
-      <c r="A627" s="8"/>
+      <c r="A627" s="4"/>
     </row>
     <row r="628">
-      <c r="A628" s="8"/>
+      <c r="A628" s="4"/>
     </row>
     <row r="629">
-      <c r="A629" s="8"/>
+      <c r="A629" s="4"/>
     </row>
     <row r="630">
-      <c r="A630" s="8"/>
+      <c r="A630" s="4"/>
     </row>
     <row r="631">
-      <c r="A631" s="8"/>
+      <c r="A631" s="4"/>
     </row>
     <row r="632">
-      <c r="A632" s="8"/>
+      <c r="A632" s="4"/>
     </row>
     <row r="633">
-      <c r="A633" s="8"/>
+      <c r="A633" s="4"/>
     </row>
     <row r="634">
-      <c r="A634" s="8"/>
+      <c r="A634" s="4"/>
     </row>
     <row r="635">
-      <c r="A635" s="8"/>
+      <c r="A635" s="4"/>
     </row>
     <row r="636">
-      <c r="A636" s="8"/>
+      <c r="A636" s="4"/>
     </row>
     <row r="637">
-      <c r="A637" s="8"/>
+      <c r="A637" s="4"/>
     </row>
     <row r="638">
-      <c r="A638" s="8"/>
+      <c r="A638" s="4"/>
     </row>
     <row r="639">
-      <c r="A639" s="8"/>
+      <c r="A639" s="4"/>
     </row>
     <row r="640">
-      <c r="A640" s="8"/>
+      <c r="A640" s="4"/>
     </row>
     <row r="641">
-      <c r="A641" s="8"/>
+      <c r="A641" s="4"/>
     </row>
     <row r="642">
-      <c r="A642" s="8"/>
+      <c r="A642" s="4"/>
     </row>
     <row r="643">
-      <c r="A643" s="8"/>
+      <c r="A643" s="4"/>
     </row>
     <row r="644">
-      <c r="A644" s="8"/>
+      <c r="A644" s="4"/>
     </row>
     <row r="645">
-      <c r="A645" s="8"/>
+      <c r="A645" s="4"/>
     </row>
     <row r="646">
-      <c r="A646" s="8"/>
+      <c r="A646" s="4"/>
     </row>
     <row r="647">
-      <c r="A647" s="8"/>
+      <c r="A647" s="4"/>
     </row>
     <row r="648">
-      <c r="A648" s="8"/>
+      <c r="A648" s="4"/>
     </row>
     <row r="649">
-      <c r="A649" s="8"/>
+      <c r="A649" s="4"/>
     </row>
     <row r="650">
-      <c r="A650" s="8"/>
+      <c r="A650" s="4"/>
     </row>
     <row r="651">
-      <c r="A651" s="8"/>
+      <c r="A651" s="4"/>
     </row>
     <row r="652">
-      <c r="A652" s="8"/>
+      <c r="A652" s="4"/>
     </row>
     <row r="653">
-      <c r="A653" s="8"/>
+      <c r="A653" s="4"/>
     </row>
     <row r="654">
-      <c r="A654" s="8"/>
+      <c r="A654" s="4"/>
     </row>
     <row r="655">
-      <c r="A655" s="8"/>
+      <c r="A655" s="4"/>
     </row>
     <row r="656">
-      <c r="A656" s="8"/>
+      <c r="A656" s="4"/>
     </row>
     <row r="657">
-      <c r="A657" s="8"/>
+      <c r="A657" s="4"/>
     </row>
     <row r="658">
-      <c r="A658" s="8"/>
+      <c r="A658" s="4"/>
     </row>
     <row r="659">
-      <c r="A659" s="8"/>
+      <c r="A659" s="4"/>
     </row>
     <row r="660">
-      <c r="A660" s="8"/>
+      <c r="A660" s="4"/>
     </row>
     <row r="661">
-      <c r="A661" s="8"/>
+      <c r="A661" s="4"/>
     </row>
     <row r="662">
-      <c r="A662" s="8"/>
+      <c r="A662" s="4"/>
     </row>
     <row r="663">
-      <c r="A663" s="8"/>
+      <c r="A663" s="4"/>
     </row>
     <row r="664">
-      <c r="A664" s="8"/>
+      <c r="A664" s="4"/>
     </row>
     <row r="665">
-      <c r="A665" s="8"/>
+      <c r="A665" s="4"/>
     </row>
     <row r="666">
-      <c r="A666" s="8"/>
+      <c r="A666" s="4"/>
     </row>
     <row r="667">
-      <c r="A667" s="8"/>
+      <c r="A667" s="4"/>
     </row>
     <row r="668">
-      <c r="A668" s="8"/>
+      <c r="A668" s="4"/>
     </row>
     <row r="669">
-      <c r="A669" s="8"/>
+      <c r="A669" s="4"/>
     </row>
     <row r="670">
-      <c r="A670" s="8"/>
+      <c r="A670" s="4"/>
     </row>
     <row r="671">
-      <c r="A671" s="8"/>
+      <c r="A671" s="4"/>
     </row>
     <row r="672">
-      <c r="A672" s="8"/>
+      <c r="A672" s="4"/>
     </row>
     <row r="673">
-      <c r="A673" s="8"/>
+      <c r="A673" s="4"/>
     </row>
     <row r="674">
-      <c r="A674" s="8"/>
+      <c r="A674" s="4"/>
     </row>
     <row r="675">
-      <c r="A675" s="8"/>
+      <c r="A675" s="4"/>
     </row>
     <row r="676">
-      <c r="A676" s="8"/>
+      <c r="A676" s="4"/>
     </row>
     <row r="677">
-      <c r="A677" s="8"/>
+      <c r="A677" s="4"/>
     </row>
     <row r="678">
-      <c r="A678" s="8"/>
+      <c r="A678" s="4"/>
     </row>
     <row r="679">
-      <c r="A679" s="8"/>
+      <c r="A679" s="4"/>
     </row>
     <row r="680">
-      <c r="A680" s="8"/>
+      <c r="A680" s="4"/>
     </row>
     <row r="681">
-      <c r="A681" s="8"/>
+      <c r="A681" s="4"/>
     </row>
     <row r="682">
-      <c r="A682" s="8"/>
+      <c r="A682" s="4"/>
     </row>
     <row r="683">
-      <c r="A683" s="8"/>
+      <c r="A683" s="4"/>
     </row>
     <row r="684">
-      <c r="A684" s="8"/>
+      <c r="A684" s="4"/>
     </row>
     <row r="685">
-      <c r="A685" s="8"/>
+      <c r="A685" s="4"/>
     </row>
     <row r="686">
-      <c r="A686" s="8"/>
+      <c r="A686" s="4"/>
     </row>
     <row r="687">
-      <c r="A687" s="8"/>
+      <c r="A687" s="4"/>
     </row>
     <row r="688">
-      <c r="A688" s="8"/>
+      <c r="A688" s="4"/>
     </row>
     <row r="689">
-      <c r="A689" s="8"/>
+      <c r="A689" s="4"/>
     </row>
     <row r="690">
-      <c r="A690" s="8"/>
+      <c r="A690" s="4"/>
     </row>
     <row r="691">
-      <c r="A691" s="8"/>
+      <c r="A691" s="4"/>
     </row>
     <row r="692">
-      <c r="A692" s="8"/>
+      <c r="A692" s="4"/>
     </row>
     <row r="693">
-      <c r="A693" s="8"/>
+      <c r="A693" s="4"/>
     </row>
     <row r="694">
-      <c r="A694" s="8"/>
+      <c r="A694" s="4"/>
     </row>
     <row r="695">
-      <c r="A695" s="8"/>
+      <c r="A695" s="4"/>
     </row>
     <row r="696">
-      <c r="A696" s="8"/>
+      <c r="A696" s="4"/>
     </row>
     <row r="697">
-      <c r="A697" s="8"/>
+      <c r="A697" s="4"/>
     </row>
     <row r="698">
-      <c r="A698" s="8"/>
+      <c r="A698" s="4"/>
     </row>
     <row r="699">
-      <c r="A699" s="8"/>
+      <c r="A699" s="4"/>
     </row>
     <row r="700">
-      <c r="A700" s="8"/>
+      <c r="A700" s="4"/>
     </row>
     <row r="701">
-      <c r="A701" s="8"/>
+      <c r="A701" s="4"/>
     </row>
     <row r="702">
-      <c r="A702" s="8"/>
+      <c r="A702" s="4"/>
     </row>
     <row r="703">
-      <c r="A703" s="8"/>
+      <c r="A703" s="4"/>
     </row>
     <row r="704">
-      <c r="A704" s="8"/>
+      <c r="A704" s="4"/>
     </row>
     <row r="705">
-      <c r="A705" s="8"/>
+      <c r="A705" s="4"/>
     </row>
     <row r="706">
-      <c r="A706" s="8"/>
+      <c r="A706" s="4"/>
     </row>
     <row r="707">
-      <c r="A707" s="8"/>
+      <c r="A707" s="4"/>
     </row>
     <row r="708">
-      <c r="A708" s="8"/>
+      <c r="A708" s="4"/>
     </row>
     <row r="709">
-      <c r="A709" s="8"/>
+      <c r="A709" s="4"/>
     </row>
     <row r="710">
-      <c r="A710" s="8"/>
+      <c r="A710" s="4"/>
     </row>
     <row r="711">
-      <c r="A711" s="8"/>
+      <c r="A711" s="4"/>
     </row>
     <row r="712">
-      <c r="A712" s="8"/>
+      <c r="A712" s="4"/>
     </row>
     <row r="713">
-      <c r="A713" s="8"/>
+      <c r="A713" s="4"/>
     </row>
     <row r="714">
-      <c r="A714" s="8"/>
+      <c r="A714" s="4"/>
     </row>
     <row r="715">
-      <c r="A715" s="8"/>
+      <c r="A715" s="4"/>
     </row>
     <row r="716">
-      <c r="A716" s="8"/>
+      <c r="A716" s="4"/>
     </row>
     <row r="717">
-      <c r="A717" s="8"/>
+      <c r="A717" s="4"/>
     </row>
     <row r="718">
-      <c r="A718" s="8"/>
+      <c r="A718" s="4"/>
     </row>
     <row r="719">
-      <c r="A719" s="8"/>
+      <c r="A719" s="4"/>
     </row>
     <row r="720">
-      <c r="A720" s="8"/>
+      <c r="A720" s="4"/>
     </row>
     <row r="721">
-      <c r="A721" s="8"/>
+      <c r="A721" s="4"/>
     </row>
     <row r="722">
-      <c r="A722" s="8"/>
+      <c r="A722" s="4"/>
     </row>
     <row r="723">
-      <c r="A723" s="8"/>
+      <c r="A723" s="4"/>
     </row>
     <row r="724">
-      <c r="A724" s="8"/>
+      <c r="A724" s="4"/>
     </row>
     <row r="725">
-      <c r="A725" s="8"/>
+      <c r="A725" s="4"/>
     </row>
     <row r="726">
-      <c r="A726" s="8"/>
+      <c r="A726" s="4"/>
     </row>
     <row r="727">
-      <c r="A727" s="8"/>
+      <c r="A727" s="4"/>
     </row>
     <row r="728">
-      <c r="A728" s="8"/>
+      <c r="A728" s="4"/>
     </row>
     <row r="729">
-      <c r="A729" s="8"/>
+      <c r="A729" s="4"/>
     </row>
     <row r="730">
-      <c r="A730" s="8"/>
+      <c r="A730" s="4"/>
     </row>
     <row r="731">
-      <c r="A731" s="8"/>
+      <c r="A731" s="4"/>
     </row>
     <row r="732">
-      <c r="A732" s="8"/>
+      <c r="A732" s="4"/>
     </row>
     <row r="733">
-      <c r="A733" s="8"/>
+      <c r="A733" s="4"/>
     </row>
     <row r="734">
-      <c r="A734" s="8"/>
+      <c r="A734" s="4"/>
     </row>
     <row r="735">
-      <c r="A735" s="8"/>
+      <c r="A735" s="4"/>
     </row>
     <row r="736">
-      <c r="A736" s="8"/>
+      <c r="A736" s="4"/>
     </row>
     <row r="737">
-      <c r="A737" s="8"/>
+      <c r="A737" s="4"/>
     </row>
     <row r="738">
-      <c r="A738" s="8"/>
+      <c r="A738" s="4"/>
     </row>
     <row r="739">
-      <c r="A739" s="8"/>
+      <c r="A739" s="4"/>
     </row>
     <row r="740">
-      <c r="A740" s="8"/>
+      <c r="A740" s="4"/>
     </row>
     <row r="741">
-      <c r="A741" s="8"/>
+      <c r="A741" s="4"/>
     </row>
     <row r="742">
-      <c r="A742" s="8"/>
+      <c r="A742" s="4"/>
     </row>
     <row r="743">
-      <c r="A743" s="8"/>
+      <c r="A743" s="4"/>
     </row>
     <row r="744">
-      <c r="A744" s="8"/>
+      <c r="A744" s="4"/>
     </row>
     <row r="745">
-      <c r="A745" s="8"/>
+      <c r="A745" s="4"/>
     </row>
     <row r="746">
-      <c r="A746" s="8"/>
+      <c r="A746" s="4"/>
     </row>
     <row r="747">
-      <c r="A747" s="8"/>
+      <c r="A747" s="4"/>
     </row>
     <row r="748">
-      <c r="A748" s="8"/>
+      <c r="A748" s="4"/>
     </row>
     <row r="749">
-      <c r="A749" s="8"/>
+      <c r="A749" s="4"/>
     </row>
     <row r="750">
-      <c r="A750" s="8"/>
+      <c r="A750" s="4"/>
     </row>
     <row r="751">
-      <c r="A751" s="8"/>
+      <c r="A751" s="4"/>
     </row>
     <row r="752">
-      <c r="A752" s="8"/>
+      <c r="A752" s="4"/>
     </row>
     <row r="753">
-      <c r="A753" s="8"/>
+      <c r="A753" s="4"/>
     </row>
     <row r="754">
-      <c r="A754" s="8"/>
+      <c r="A754" s="4"/>
     </row>
     <row r="755">
-      <c r="A755" s="8"/>
+      <c r="A755" s="4"/>
     </row>
     <row r="756">
-      <c r="A756" s="8"/>
+      <c r="A756" s="4"/>
     </row>
     <row r="757">
-      <c r="A757" s="8"/>
+      <c r="A757" s="4"/>
     </row>
     <row r="758">
-      <c r="A758" s="8"/>
+      <c r="A758" s="4"/>
     </row>
     <row r="759">
-      <c r="A759" s="8"/>
+      <c r="A759" s="4"/>
     </row>
     <row r="760">
-      <c r="A760" s="8"/>
+      <c r="A760" s="4"/>
     </row>
     <row r="761">
-      <c r="A761" s="8"/>
+      <c r="A761" s="4"/>
     </row>
     <row r="762">
-      <c r="A762" s="8"/>
+      <c r="A762" s="4"/>
     </row>
     <row r="763">
-      <c r="A763" s="8"/>
+      <c r="A763" s="4"/>
     </row>
     <row r="764">
-      <c r="A764" s="8"/>
+      <c r="A764" s="4"/>
     </row>
     <row r="765">
-      <c r="A765" s="8"/>
+      <c r="A765" s="4"/>
     </row>
     <row r="766">
-      <c r="A766" s="8"/>
+      <c r="A766" s="4"/>
     </row>
     <row r="767">
-      <c r="A767" s="8"/>
+      <c r="A767" s="4"/>
     </row>
     <row r="768">
-      <c r="A768" s="8"/>
+      <c r="A768" s="4"/>
     </row>
     <row r="769">
-      <c r="A769" s="8"/>
+      <c r="A769" s="4"/>
     </row>
     <row r="770">
-      <c r="A770" s="8"/>
+      <c r="A770" s="4"/>
     </row>
     <row r="771">
-      <c r="A771" s="8"/>
+      <c r="A771" s="4"/>
     </row>
     <row r="772">
-      <c r="A772" s="8"/>
+      <c r="A772" s="4"/>
     </row>
     <row r="773">
-      <c r="A773" s="8"/>
+      <c r="A773" s="4"/>
     </row>
     <row r="774">
-      <c r="A774" s="8"/>
+      <c r="A774" s="4"/>
     </row>
     <row r="775">
-      <c r="A775" s="8"/>
+      <c r="A775" s="4"/>
     </row>
     <row r="776">
-      <c r="A776" s="8"/>
+      <c r="A776" s="4"/>
     </row>
     <row r="777">
-      <c r="A777" s="8"/>
+      <c r="A777" s="4"/>
     </row>
     <row r="778">
-      <c r="A778" s="8"/>
+      <c r="A778" s="4"/>
     </row>
     <row r="779">
-      <c r="A779" s="8"/>
+      <c r="A779" s="4"/>
     </row>
     <row r="780">
-      <c r="A780" s="8"/>
+      <c r="A780" s="4"/>
     </row>
     <row r="781">
-      <c r="A781" s="8"/>
+      <c r="A781" s="4"/>
     </row>
     <row r="782">
-      <c r="A782" s="8"/>
+      <c r="A782" s="4"/>
     </row>
     <row r="783">
-      <c r="A783" s="8"/>
+      <c r="A783" s="4"/>
     </row>
     <row r="784">
-      <c r="A784" s="8"/>
+      <c r="A784" s="4"/>
     </row>
     <row r="785">
-      <c r="A785" s="8"/>
+      <c r="A785" s="4"/>
     </row>
     <row r="786">
-      <c r="A786" s="8"/>
+      <c r="A786" s="4"/>
     </row>
     <row r="787">
-      <c r="A787" s="8"/>
+      <c r="A787" s="4"/>
     </row>
     <row r="788">
-      <c r="A788" s="8"/>
+      <c r="A788" s="4"/>
     </row>
     <row r="789">
-      <c r="A789" s="8"/>
+      <c r="A789" s="4"/>
     </row>
     <row r="790">
-      <c r="A790" s="8"/>
+      <c r="A790" s="4"/>
     </row>
     <row r="791">
-      <c r="A791" s="8"/>
+      <c r="A791" s="4"/>
     </row>
     <row r="792">
-      <c r="A792" s="8"/>
+      <c r="A792" s="4"/>
     </row>
     <row r="793">
-      <c r="A793" s="8"/>
+      <c r="A793" s="4"/>
     </row>
     <row r="794">
-      <c r="A794" s="8"/>
+      <c r="A794" s="4"/>
     </row>
     <row r="795">
-      <c r="A795" s="8"/>
+      <c r="A795" s="4"/>
     </row>
     <row r="796">
-      <c r="A796" s="8"/>
+      <c r="A796" s="4"/>
     </row>
     <row r="797">
-      <c r="A797" s="8"/>
+      <c r="A797" s="4"/>
     </row>
     <row r="798">
-      <c r="A798" s="8"/>
+      <c r="A798" s="4"/>
     </row>
     <row r="799">
-      <c r="A799" s="8"/>
+      <c r="A799" s="4"/>
     </row>
     <row r="800">
-      <c r="A800" s="8"/>
+      <c r="A800" s="4"/>
     </row>
     <row r="801">
-      <c r="A801" s="8"/>
+      <c r="A801" s="4"/>
     </row>
     <row r="802">
-      <c r="A802" s="8"/>
+      <c r="A802" s="4"/>
     </row>
     <row r="803">
-      <c r="A803" s="8"/>
+      <c r="A803" s="4"/>
     </row>
     <row r="804">
-      <c r="A804" s="8"/>
+      <c r="A804" s="4"/>
     </row>
     <row r="805">
-      <c r="A805" s="8"/>
+      <c r="A805" s="4"/>
     </row>
     <row r="806">
-      <c r="A806" s="8"/>
+      <c r="A806" s="4"/>
     </row>
     <row r="807">
-      <c r="A807" s="8"/>
+      <c r="A807" s="4"/>
     </row>
     <row r="808">
-      <c r="A808" s="8"/>
+      <c r="A808" s="4"/>
     </row>
     <row r="809">
-      <c r="A809" s="8"/>
+      <c r="A809" s="4"/>
     </row>
     <row r="810">
-      <c r="A810" s="8"/>
+      <c r="A810" s="4"/>
     </row>
     <row r="811">
-      <c r="A811" s="8"/>
+      <c r="A811" s="4"/>
     </row>
     <row r="812">
-      <c r="A812" s="8"/>
+      <c r="A812" s="4"/>
     </row>
     <row r="813">
-      <c r="A813" s="8"/>
+      <c r="A813" s="4"/>
     </row>
     <row r="814">
-      <c r="A814" s="8"/>
+      <c r="A814" s="4"/>
     </row>
     <row r="815">
-      <c r="A815" s="8"/>
+      <c r="A815" s="4"/>
     </row>
     <row r="816">
-      <c r="A816" s="8"/>
+      <c r="A816" s="4"/>
     </row>
     <row r="817">
-      <c r="A817" s="8"/>
+      <c r="A817" s="4"/>
     </row>
     <row r="818">
-      <c r="A818" s="8"/>
+      <c r="A818" s="4"/>
     </row>
     <row r="819">
-      <c r="A819" s="8"/>
+      <c r="A819" s="4"/>
     </row>
     <row r="820">
-      <c r="A820" s="8"/>
+      <c r="A820" s="4"/>
     </row>
     <row r="821">
-      <c r="A821" s="8"/>
+      <c r="A821" s="4"/>
     </row>
     <row r="822">
-      <c r="A822" s="8"/>
+      <c r="A822" s="4"/>
     </row>
     <row r="823">
-      <c r="A823" s="8"/>
+      <c r="A823" s="4"/>
     </row>
     <row r="824">
-      <c r="A824" s="8"/>
+      <c r="A824" s="4"/>
     </row>
     <row r="825">
-      <c r="A825" s="8"/>
+      <c r="A825" s="4"/>
     </row>
     <row r="826">
-      <c r="A826" s="8"/>
+      <c r="A826" s="4"/>
     </row>
     <row r="827">
-      <c r="A827" s="8"/>
+      <c r="A827" s="4"/>
     </row>
     <row r="828">
-      <c r="A828" s="8"/>
+      <c r="A828" s="4"/>
     </row>
     <row r="829">
-      <c r="A829" s="8"/>
+      <c r="A829" s="4"/>
     </row>
     <row r="830">
-      <c r="A830" s="8"/>
+      <c r="A830" s="4"/>
     </row>
     <row r="831">
-      <c r="A831" s="8"/>
+      <c r="A831" s="4"/>
     </row>
     <row r="832">
-      <c r="A832" s="8"/>
+      <c r="A832" s="4"/>
     </row>
     <row r="833">
-      <c r="A833" s="8"/>
+      <c r="A833" s="4"/>
     </row>
     <row r="834">
-      <c r="A834" s="8"/>
+      <c r="A834" s="4"/>
     </row>
     <row r="835">
-      <c r="A835" s="8"/>
+      <c r="A835" s="4"/>
     </row>
     <row r="836">
-      <c r="A836" s="8"/>
+      <c r="A836" s="4"/>
     </row>
     <row r="837">
-      <c r="A837" s="8"/>
+      <c r="A837" s="4"/>
     </row>
     <row r="838">
-      <c r="A838" s="8"/>
+      <c r="A838" s="4"/>
     </row>
     <row r="839">
-      <c r="A839" s="8"/>
+      <c r="A839" s="4"/>
     </row>
     <row r="840">
-      <c r="A840" s="8"/>
+      <c r="A840" s="4"/>
     </row>
     <row r="841">
-      <c r="A841" s="8"/>
+      <c r="A841" s="4"/>
     </row>
     <row r="842">
-      <c r="A842" s="8"/>
+      <c r="A842" s="4"/>
     </row>
     <row r="843">
-      <c r="A843" s="8"/>
+      <c r="A843" s="4"/>
     </row>
     <row r="844">
-      <c r="A844" s="8"/>
+      <c r="A844" s="4"/>
     </row>
     <row r="845">
-      <c r="A845" s="8"/>
+      <c r="A845" s="4"/>
     </row>
     <row r="846">
-      <c r="A846" s="8"/>
+      <c r="A846" s="4"/>
     </row>
     <row r="847">
-      <c r="A847" s="8"/>
+      <c r="A847" s="4"/>
     </row>
     <row r="848">
-      <c r="A848" s="8"/>
+      <c r="A848" s="4"/>
     </row>
     <row r="849">
-      <c r="A849" s="8"/>
+      <c r="A849" s="4"/>
     </row>
     <row r="850">
-      <c r="A850" s="8"/>
+      <c r="A850" s="4"/>
     </row>
     <row r="851">
-      <c r="A851" s="8"/>
+      <c r="A851" s="4"/>
     </row>
     <row r="852">
-      <c r="A852" s="8"/>
+      <c r="A852" s="4"/>
     </row>
     <row r="853">
-      <c r="A853" s="8"/>
+      <c r="A853" s="4"/>
     </row>
     <row r="854">
-      <c r="A854" s="8"/>
+      <c r="A854" s="4"/>
     </row>
     <row r="855">
-      <c r="A855" s="8"/>
+      <c r="A855" s="4"/>
     </row>
     <row r="856">
-      <c r="A856" s="8"/>
+      <c r="A856" s="4"/>
     </row>
     <row r="857">
-      <c r="A857" s="8"/>
+      <c r="A857" s="4"/>
     </row>
     <row r="858">
-      <c r="A858" s="8"/>
+      <c r="A858" s="4"/>
     </row>
     <row r="859">
-      <c r="A859" s="8"/>
+      <c r="A859" s="4"/>
     </row>
     <row r="860">
-      <c r="A860" s="8"/>
+      <c r="A860" s="4"/>
     </row>
     <row r="861">
-      <c r="A861" s="8"/>
+      <c r="A861" s="4"/>
     </row>
     <row r="862">
-      <c r="A862" s="8"/>
+      <c r="A862" s="4"/>
     </row>
     <row r="863">
-      <c r="A863" s="8"/>
+      <c r="A863" s="4"/>
     </row>
     <row r="864">
-      <c r="A864" s="8"/>
+      <c r="A864" s="4"/>
     </row>
     <row r="865">
-      <c r="A865" s="8"/>
+      <c r="A865" s="4"/>
     </row>
     <row r="866">
-      <c r="A866" s="8"/>
+      <c r="A866" s="4"/>
     </row>
     <row r="867">
-      <c r="A867" s="8"/>
+      <c r="A867" s="4"/>
     </row>
     <row r="868">
-      <c r="A868" s="8"/>
+      <c r="A868" s="4"/>
     </row>
     <row r="869">
-      <c r="A869" s="8"/>
+      <c r="A869" s="4"/>
     </row>
     <row r="870">
-      <c r="A870" s="8"/>
+      <c r="A870" s="4"/>
     </row>
     <row r="871">
-      <c r="A871" s="8"/>
+      <c r="A871" s="4"/>
     </row>
     <row r="872">
-      <c r="A872" s="8"/>
+      <c r="A872" s="4"/>
     </row>
     <row r="873">
-      <c r="A873" s="8"/>
+      <c r="A873" s="4"/>
     </row>
     <row r="874">
-      <c r="A874" s="8"/>
+      <c r="A874" s="4"/>
     </row>
     <row r="875">
-      <c r="A875" s="8"/>
+      <c r="A875" s="4"/>
     </row>
     <row r="876">
-      <c r="A876" s="8"/>
+      <c r="A876" s="4"/>
     </row>
     <row r="877">
-      <c r="A877" s="8"/>
+      <c r="A877" s="4"/>
     </row>
     <row r="878">
-      <c r="A878" s="8"/>
+      <c r="A878" s="4"/>
     </row>
     <row r="879">
-      <c r="A879" s="8"/>
+      <c r="A879" s="4"/>
     </row>
     <row r="880">
-      <c r="A880" s="8"/>
+      <c r="A880" s="4"/>
     </row>
     <row r="881">
-      <c r="A881" s="8"/>
+      <c r="A881" s="4"/>
     </row>
     <row r="882">
-      <c r="A882" s="8"/>
+      <c r="A882" s="4"/>
     </row>
     <row r="883">
-      <c r="A883" s="8"/>
+      <c r="A883" s="4"/>
     </row>
     <row r="884">
-      <c r="A884" s="8"/>
+      <c r="A884" s="4"/>
     </row>
     <row r="885">
-      <c r="A885" s="8"/>
+      <c r="A885" s="4"/>
     </row>
     <row r="886">
-      <c r="A886" s="8"/>
+      <c r="A886" s="4"/>
     </row>
     <row r="887">
-      <c r="A887" s="8"/>
+      <c r="A887" s="4"/>
     </row>
     <row r="888">
-      <c r="A888" s="8"/>
+      <c r="A888" s="4"/>
     </row>
     <row r="889">
-      <c r="A889" s="8"/>
+      <c r="A889" s="4"/>
     </row>
     <row r="890">
-      <c r="A890" s="8"/>
+      <c r="A890" s="4"/>
     </row>
     <row r="891">
-      <c r="A891" s="8"/>
+      <c r="A891" s="4"/>
     </row>
     <row r="892">
-      <c r="A892" s="8"/>
+      <c r="A892" s="4"/>
     </row>
     <row r="893">
-      <c r="A893" s="8"/>
+      <c r="A893" s="4"/>
     </row>
     <row r="894">
-      <c r="A894" s="8"/>
+      <c r="A894" s="4"/>
     </row>
     <row r="895">
-      <c r="A895" s="8"/>
+      <c r="A895" s="4"/>
     </row>
     <row r="896">
-      <c r="A896" s="8"/>
+      <c r="A896" s="4"/>
     </row>
     <row r="897">
-      <c r="A897" s="8"/>
+      <c r="A897" s="4"/>
     </row>
     <row r="898">
-      <c r="A898" s="8"/>
+      <c r="A898" s="4"/>
     </row>
     <row r="899">
-      <c r="A899" s="8"/>
+      <c r="A899" s="4"/>
     </row>
     <row r="900">
-      <c r="A900" s="8"/>
+      <c r="A900" s="4"/>
     </row>
     <row r="901">
-      <c r="A901" s="8"/>
+      <c r="A901" s="4"/>
     </row>
     <row r="902">
-      <c r="A902" s="8"/>
+      <c r="A902" s="4"/>
     </row>
     <row r="903">
-      <c r="A903" s="8"/>
+      <c r="A903" s="4"/>
     </row>
     <row r="904">
-      <c r="A904" s="8"/>
+      <c r="A904" s="4"/>
     </row>
     <row r="905">
-      <c r="A905" s="8"/>
+      <c r="A905" s="4"/>
     </row>
     <row r="906">
-      <c r="A906" s="8"/>
+      <c r="A906" s="4"/>
     </row>
     <row r="907">
-      <c r="A907" s="8"/>
+      <c r="A907" s="4"/>
     </row>
     <row r="908">
-      <c r="A908" s="8"/>
+      <c r="A908" s="4"/>
     </row>
     <row r="909">
-      <c r="A909" s="8"/>
+      <c r="A909" s="4"/>
     </row>
     <row r="910">
-      <c r="A910" s="8"/>
+      <c r="A910" s="4"/>
     </row>
     <row r="911">
-      <c r="A911" s="8"/>
+      <c r="A911" s="4"/>
     </row>
     <row r="912">
-      <c r="A912" s="8"/>
+      <c r="A912" s="4"/>
     </row>
     <row r="913">
-      <c r="A913" s="8"/>
+      <c r="A913" s="4"/>
     </row>
     <row r="914">
-      <c r="A914" s="8"/>
+      <c r="A914" s="4"/>
     </row>
     <row r="915">
-      <c r="A915" s="8"/>
+      <c r="A915" s="4"/>
     </row>
     <row r="916">
-      <c r="A916" s="8"/>
+      <c r="A916" s="4"/>
     </row>
     <row r="917">
-      <c r="A917" s="8"/>
+      <c r="A917" s="4"/>
     </row>
     <row r="918">
-      <c r="A918" s="8"/>
+      <c r="A918" s="4"/>
     </row>
     <row r="919">
-      <c r="A919" s="8"/>
+      <c r="A919" s="4"/>
     </row>
     <row r="920">
-      <c r="A920" s="8"/>
+      <c r="A920" s="4"/>
     </row>
     <row r="921">
-      <c r="A921" s="8"/>
+      <c r="A921" s="4"/>
     </row>
     <row r="922">
-      <c r="A922" s="8"/>
+      <c r="A922" s="4"/>
     </row>
     <row r="923">
-      <c r="A923" s="8"/>
+      <c r="A923" s="4"/>
     </row>
     <row r="924">
-      <c r="A924" s="8"/>
+      <c r="A924" s="4"/>
     </row>
     <row r="925">
-      <c r="A925" s="8"/>
+      <c r="A925" s="4"/>
     </row>
     <row r="926">
-      <c r="A926" s="8"/>
+      <c r="A926" s="4"/>
     </row>
     <row r="927">
-      <c r="A927" s="8"/>
+      <c r="A927" s="4"/>
     </row>
     <row r="928">
-      <c r="A928" s="8"/>
+      <c r="A928" s="4"/>
     </row>
     <row r="929">
-      <c r="A929" s="8"/>
+      <c r="A929" s="4"/>
     </row>
     <row r="930">
-      <c r="A930" s="8"/>
+      <c r="A930" s="4"/>
     </row>
     <row r="931">
-      <c r="A931" s="8"/>
+      <c r="A931" s="4"/>
     </row>
     <row r="932">
-      <c r="A932" s="8"/>
+      <c r="A932" s="4"/>
     </row>
     <row r="933">
-      <c r="A933" s="8"/>
+      <c r="A933" s="4"/>
     </row>
     <row r="934">
-      <c r="A934" s="8"/>
+      <c r="A934" s="4"/>
     </row>
     <row r="935">
-      <c r="A935" s="8"/>
+      <c r="A935" s="4"/>
     </row>
     <row r="936">
-      <c r="A936" s="8"/>
+      <c r="A936" s="4"/>
     </row>
     <row r="937">
-      <c r="A937" s="8"/>
+      <c r="A937" s="4"/>
     </row>
     <row r="938">
-      <c r="A938" s="8"/>
+      <c r="A938" s="4"/>
     </row>
     <row r="939">
-      <c r="A939" s="8"/>
+      <c r="A939" s="4"/>
     </row>
     <row r="940">
-      <c r="A940" s="8"/>
+      <c r="A940" s="4"/>
     </row>
     <row r="941">
-      <c r="A941" s="8"/>
+      <c r="A941" s="4"/>
     </row>
     <row r="942">
-      <c r="A942" s="8"/>
+      <c r="A942" s="4"/>
     </row>
     <row r="943">
-      <c r="A943" s="8"/>
+      <c r="A943" s="4"/>
     </row>
     <row r="944">
-      <c r="A944" s="8"/>
+      <c r="A944" s="4"/>
     </row>
     <row r="945">
-      <c r="A945" s="8"/>
+      <c r="A945" s="4"/>
     </row>
     <row r="946">
-      <c r="A946" s="8"/>
+      <c r="A946" s="4"/>
     </row>
     <row r="947">
-      <c r="A947" s="8"/>
+      <c r="A947" s="4"/>
     </row>
     <row r="948">
-      <c r="A948" s="8"/>
+      <c r="A948" s="4"/>
     </row>
     <row r="949">
-      <c r="A949" s="8"/>
+      <c r="A949" s="4"/>
     </row>
     <row r="950">
-      <c r="A950" s="8"/>
+      <c r="A950" s="4"/>
     </row>
     <row r="951">
-      <c r="A951" s="8"/>
+      <c r="A951" s="4"/>
     </row>
     <row r="952">
-      <c r="A952" s="8"/>
+      <c r="A952" s="4"/>
     </row>
     <row r="953">
-      <c r="A953" s="8"/>
+      <c r="A953" s="4"/>
     </row>
     <row r="954">
-      <c r="A954" s="8"/>
+      <c r="A954" s="4"/>
     </row>
     <row r="955">
-      <c r="A955" s="8"/>
+      <c r="A955" s="4"/>
     </row>
     <row r="956">
-      <c r="A956" s="8"/>
+      <c r="A956" s="4"/>
     </row>
     <row r="957">
-      <c r="A957" s="8"/>
+      <c r="A957" s="4"/>
     </row>
     <row r="958">
-      <c r="A958" s="8"/>
+      <c r="A958" s="4"/>
     </row>
     <row r="959">
-      <c r="A959" s="8"/>
+      <c r="A959" s="4"/>
     </row>
     <row r="960">
-      <c r="A960" s="8"/>
+      <c r="A960" s="4"/>
     </row>
     <row r="961">
-      <c r="A961" s="8"/>
+      <c r="A961" s="4"/>
     </row>
     <row r="962">
-      <c r="A962" s="8"/>
+      <c r="A962" s="4"/>
     </row>
     <row r="963">
-      <c r="A963" s="8"/>
+      <c r="A963" s="4"/>
     </row>
     <row r="964">
-      <c r="A964" s="8"/>
+      <c r="A964" s="4"/>
     </row>
     <row r="965">
-      <c r="A965" s="8"/>
+      <c r="A965" s="4"/>
     </row>
     <row r="966">
-      <c r="A966" s="8"/>
+      <c r="A966" s="4"/>
     </row>
     <row r="967">
-      <c r="A967" s="8"/>
+      <c r="A967" s="4"/>
     </row>
     <row r="968">
-      <c r="A968" s="8"/>
+      <c r="A968" s="4"/>
     </row>
     <row r="969">
-      <c r="A969" s="8"/>
+      <c r="A969" s="4"/>
     </row>
     <row r="970">
-      <c r="A970" s="8"/>
+      <c r="A970" s="4"/>
     </row>
     <row r="971">
-      <c r="A971" s="8"/>
+      <c r="A971" s="4"/>
     </row>
     <row r="972">
-      <c r="A972" s="8"/>
+      <c r="A972" s="4"/>
     </row>
     <row r="973">
-      <c r="A973" s="8"/>
+      <c r="A973" s="4"/>
     </row>
     <row r="974">
-      <c r="A974" s="8"/>
+      <c r="A974" s="4"/>
     </row>
     <row r="975">
-      <c r="A975" s="8"/>
+      <c r="A975" s="4"/>
     </row>
     <row r="976">
-      <c r="A976" s="8"/>
-    </row>
-    <row r="977">
-      <c r="A977" s="8"/>
-    </row>
-    <row r="978">
-      <c r="A978" s="8"/>
-    </row>
-    <row r="979">
-      <c r="A979" s="8"/>
-    </row>
-    <row r="980">
-      <c r="A980" s="8"/>
-    </row>
-    <row r="981">
-      <c r="A981" s="8"/>
-    </row>
-    <row r="982">
-      <c r="A982" s="8"/>
-    </row>
-    <row r="983">
-      <c r="A983" s="8"/>
-    </row>
-    <row r="984">
-      <c r="A984" s="8"/>
-    </row>
-    <row r="985">
-      <c r="A985" s="8"/>
-    </row>
-    <row r="986">
-      <c r="A986" s="8"/>
-    </row>
-    <row r="987">
-      <c r="A987" s="8"/>
+      <c r="A976" s="4"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Add new excel attendees
</commit_message>
<xml_diff>
--- a/images/Attendee Companies Con-X 2022.xlsx
+++ b/images/Attendee Companies Con-X 2022.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>A2 Secure</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Allbeds</t>
   </si>
   <si>
-    <t>Allresnet (Alliance Reservations)</t>
+    <t>Altostratus Cloud Consulting</t>
   </si>
   <si>
     <t>Altura Destination Services</t>
@@ -58,19 +58,13 @@
     <t>Aurumtours</t>
   </si>
   <si>
-    <t>Avoris</t>
-  </si>
-  <si>
-    <t>Azabache</t>
+    <t>Avoris Travel</t>
   </si>
   <si>
     <t>Barcelo Hotel Group</t>
   </si>
   <si>
-    <t>BAVEL-VOXEL GROUP</t>
-  </si>
-  <si>
-    <t>BD Director</t>
+    <t>Baxel-Voxel Group</t>
   </si>
   <si>
     <t>Bd4 travel</t>
@@ -91,6 +85,9 @@
     <t>BG Hotels</t>
   </si>
   <si>
+    <t>bhollyconsulting.com</t>
+  </si>
+  <si>
     <t>Blau Hotels &amp; Resorts</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
     <t>Carthage Group</t>
   </si>
   <si>
+    <t>Central de Reservas</t>
+  </si>
+  <si>
     <t>Clicktrip</t>
   </si>
   <si>
@@ -133,22 +133,22 @@
     <t>DerbySoft</t>
   </si>
   <si>
+    <t>Despegar/Hoteldo</t>
+  </si>
+  <si>
     <t>Dida Travel</t>
   </si>
   <si>
     <t>Dieux Travel Service</t>
   </si>
   <si>
-    <t>Director of BD</t>
-  </si>
-  <si>
     <t>Doctorwhatson</t>
   </si>
   <si>
     <t>Easy Market</t>
   </si>
   <si>
-    <t>El Corte Inglès</t>
+    <t>eDreams</t>
   </si>
   <si>
     <t>Emerging Travel</t>
@@ -172,10 +172,13 @@
     <t>Expedia Partner Solutions</t>
   </si>
   <si>
+    <t>Fastly</t>
+  </si>
+  <si>
     <t>Fastpayhotels</t>
   </si>
   <si>
-    <t xml:space="preserve">FDSA </t>
+    <t>FDSA</t>
   </si>
   <si>
     <t>FI iniciativas</t>
@@ -184,7 +187,7 @@
     <t>FindHotel</t>
   </si>
   <si>
-    <t>Founder</t>
+    <t>FTI Touristik GmbH</t>
   </si>
   <si>
     <t>G2 Travel</t>
@@ -223,7 +226,7 @@
     <t>Hosteltur.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Hotelbeds </t>
+    <t>Hotelbeds</t>
   </si>
   <si>
     <t>HotelDO / Despegar</t>
@@ -265,10 +268,7 @@
     <t>Imperatore Travel</t>
   </si>
   <si>
-    <t>INFINITE HOTEL</t>
-  </si>
-  <si>
-    <t>Intuitive systems</t>
+    <t>Infinite Hotels</t>
   </si>
   <si>
     <t>iTravex</t>
@@ -277,9 +277,6 @@
     <t>Jacobs Media Group</t>
   </si>
   <si>
-    <t>JTB Global Marketing &amp; Travel</t>
-  </si>
-  <si>
     <t>Jumbo Tours</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>Karavel</t>
   </si>
   <si>
-    <t>KAYAK</t>
-  </si>
-  <si>
     <t>Keytours Vacations</t>
   </si>
   <si>
@@ -310,12 +304,18 @@
     <t>Kyte</t>
   </si>
   <si>
-    <t xml:space="preserve">LAlianxa </t>
-  </si>
-  <si>
     <t>Logitravel</t>
   </si>
   <si>
+    <t>Mabrian Technologies</t>
+  </si>
+  <si>
+    <t>Magic Breaks</t>
+  </si>
+  <si>
+    <t>Melia</t>
+  </si>
+  <si>
     <t>Methabook</t>
   </si>
   <si>
@@ -343,6 +343,9 @@
     <t>Nemo Group</t>
   </si>
   <si>
+    <t>Netstorming</t>
+  </si>
+  <si>
     <t>Nezasa</t>
   </si>
   <si>
@@ -358,16 +361,22 @@
     <t>Offtryp</t>
   </si>
   <si>
+    <t>OH-TEC</t>
+  </si>
+  <si>
     <t>On the Beach</t>
   </si>
   <si>
+    <t>One Up Travel</t>
+  </si>
+  <si>
     <t>OnTravel</t>
   </si>
   <si>
     <t>Open Destinations</t>
   </si>
   <si>
-    <t>Ostrovok</t>
+    <t>OpenRooms</t>
   </si>
   <si>
     <t>OTS Globe</t>
@@ -415,6 +424,9 @@
     <t>RateTiger</t>
   </si>
   <si>
+    <t>Resort Marketing International</t>
+  </si>
+  <si>
     <t>Roibos</t>
   </si>
   <si>
@@ -424,7 +436,7 @@
     <t>roomsXXL</t>
   </si>
   <si>
-    <t>Roxa Hospitality</t>
+    <t>Restel</t>
   </si>
   <si>
     <t>Sandals</t>
@@ -463,9 +475,6 @@
     <t>Spain Top</t>
   </si>
   <si>
-    <t>Splitty - Holisto</t>
-  </si>
-  <si>
     <t>Sriggle</t>
   </si>
   <si>
@@ -496,10 +505,7 @@
     <t>The Hub4Travel</t>
   </si>
   <si>
-    <t>The Travel hub - tthtravel.net</t>
-  </si>
-  <si>
-    <t>The travel junction (Flight Centre)</t>
+    <t>Thinklithe</t>
   </si>
   <si>
     <t>Thomas Cook</t>
@@ -514,19 +520,19 @@
     <t>Travel Weekly Group</t>
   </si>
   <si>
-    <t>traveltek</t>
+    <t>Traveltek</t>
   </si>
   <si>
     <t>TravelUp</t>
   </si>
   <si>
-    <t>Travelxchange</t>
-  </si>
-  <si>
     <t>Travolution</t>
   </si>
   <si>
-    <t>Trip.com</t>
+    <t>Travtravel</t>
+  </si>
+  <si>
+    <t>Trip.com Group</t>
   </si>
   <si>
     <t>Tripx Travel AB</t>
@@ -547,13 +553,10 @@
     <t>Veri Seed Capital</t>
   </si>
   <si>
-    <t>Vervotech</t>
-  </si>
-  <si>
     <t>Viajes El Corte Ingles</t>
   </si>
   <si>
-    <t>VIAJES INTERRIAS</t>
+    <t>Viajes Interrias</t>
   </si>
   <si>
     <t>Viajes Olympia</t>
@@ -611,7 +614,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -619,6 +622,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF666666"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11.0"/>
       <color rgb="FF666666"/>
       <name val="Roboto"/>
@@ -644,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -660,6 +669,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -971,12 +983,12 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -986,12 +998,12 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1001,7 +1013,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1011,7 +1023,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1091,17 +1103,17 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1116,7 +1128,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1161,7 +1173,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1176,7 +1188,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1191,12 +1203,12 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1211,57 +1223,57 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1271,12 +1283,12 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1291,12 +1303,12 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1316,7 +1328,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1341,12 +1353,12 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1356,7 +1368,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="8" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1366,7 +1378,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1376,7 +1388,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1431,7 +1443,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="7" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1456,12 +1468,12 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="4" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1471,7 +1483,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1481,17 +1493,17 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1506,32 +1518,32 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1551,7 +1563,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1566,7 +1578,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1586,7 +1598,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="7" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1596,12 +1608,12 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="5" t="s">
+      <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1611,22 +1623,22 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="2" t="s">
+      <c r="A147" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1636,7 +1648,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="3" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1646,12 +1658,12 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="8" t="s">
+      <c r="A153" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1666,12 +1678,12 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="9" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="5" t="s">
+      <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1681,12 +1693,12 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="7" t="s">
+      <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="2" t="s">
+      <c r="A160" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1696,17 +1708,17 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="5" t="s">
+      <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1716,27 +1728,27 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="5" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="4" t="s">
+      <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="4" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="5" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1746,7 +1758,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="6" t="s">
+      <c r="A172" s="3" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1756,7 +1768,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1766,7 +1778,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="4" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1781,42 +1793,42 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="4" t="s">
+      <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="2" t="s">
+      <c r="A181" s="4" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="5" t="s">
+      <c r="A182" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="5" t="s">
+      <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="2" t="s">
+      <c r="A186" s="5" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1826,27 +1838,27 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="1" t="s">
+      <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="4" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="3" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1856,12 +1868,12 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="6" t="s">
+      <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="2" t="s">
+      <c r="A195" s="7" t="s">
         <v>194</v>
       </c>
     </row>
@@ -1871,17 +1883,19 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="4" t="s">
+      <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="4" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="4"/>
+      <c r="A199" s="2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="4"/>
@@ -4112,112 +4126,13 @@
     <row r="942">
       <c r="A942" s="4"/>
     </row>
-    <row r="943">
-      <c r="A943" s="4"/>
-    </row>
-    <row r="944">
-      <c r="A944" s="4"/>
-    </row>
-    <row r="945">
-      <c r="A945" s="4"/>
-    </row>
-    <row r="946">
-      <c r="A946" s="4"/>
-    </row>
-    <row r="947">
-      <c r="A947" s="4"/>
-    </row>
-    <row r="948">
-      <c r="A948" s="4"/>
-    </row>
-    <row r="949">
-      <c r="A949" s="4"/>
-    </row>
-    <row r="950">
-      <c r="A950" s="4"/>
-    </row>
-    <row r="951">
-      <c r="A951" s="4"/>
-    </row>
-    <row r="952">
-      <c r="A952" s="4"/>
-    </row>
-    <row r="953">
-      <c r="A953" s="4"/>
-    </row>
-    <row r="954">
-      <c r="A954" s="4"/>
-    </row>
-    <row r="955">
-      <c r="A955" s="4"/>
-    </row>
-    <row r="956">
-      <c r="A956" s="4"/>
-    </row>
-    <row r="957">
-      <c r="A957" s="4"/>
-    </row>
-    <row r="958">
-      <c r="A958" s="4"/>
-    </row>
-    <row r="959">
-      <c r="A959" s="4"/>
-    </row>
-    <row r="960">
-      <c r="A960" s="4"/>
-    </row>
-    <row r="961">
-      <c r="A961" s="4"/>
-    </row>
-    <row r="962">
-      <c r="A962" s="4"/>
-    </row>
-    <row r="963">
-      <c r="A963" s="4"/>
-    </row>
-    <row r="964">
-      <c r="A964" s="4"/>
-    </row>
-    <row r="965">
-      <c r="A965" s="4"/>
-    </row>
-    <row r="966">
-      <c r="A966" s="4"/>
-    </row>
-    <row r="967">
-      <c r="A967" s="4"/>
-    </row>
-    <row r="968">
-      <c r="A968" s="4"/>
-    </row>
-    <row r="969">
-      <c r="A969" s="4"/>
-    </row>
-    <row r="970">
-      <c r="A970" s="4"/>
-    </row>
-    <row r="971">
-      <c r="A971" s="4"/>
-    </row>
-    <row r="972">
-      <c r="A972" s="4"/>
-    </row>
-    <row r="973">
-      <c r="A973" s="4"/>
-    </row>
-    <row r="974">
-      <c r="A974" s="4"/>
-    </row>
-    <row r="975">
-      <c r="A975" s="4"/>
-    </row>
-    <row r="976">
-      <c r="A976" s="4"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A25"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" orientation="portrait" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>